<commit_message>
tagged ~60 facebook posts
</commit_message>
<xml_diff>
--- a/data_utils/data_for_tagging.xlsx
+++ b/data_utils/data_for_tagging.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Y\PycharmProjects\traveliz\data_utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eliyasegev/PycharmProjects/traveliz/data_utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{D369A063-D92F-40D9-B1A2-B5BDF3EAF5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="facebook_posts_1" sheetId="1" r:id="rId1"/>
@@ -18,13 +17,20 @@
     <sheet name="facebook_posts_3" sheetId="3" r:id="rId3"/>
     <sheet name="facebook_posts_4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1730" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1675" uniqueCount="510">
   <si>
     <t>Post_id</t>
   </si>
@@ -2480,11 +2486,269 @@
   <si>
     <t>יפו</t>
   </si>
+  <si>
+    <t>06.1.2022</t>
+  </si>
+  <si>
+    <t>31.03.2022</t>
+  </si>
+  <si>
+    <t>תל אביב</t>
+  </si>
+  <si>
+    <t>ירושלים</t>
+  </si>
+  <si>
+    <t>עמק החולה</t>
+  </si>
+  <si>
+    <t>21.11.2021</t>
+  </si>
+  <si>
+    <t>24.11.2021</t>
+  </si>
+  <si>
+    <t>פרדס חנה</t>
+  </si>
+  <si>
+    <t>חולתה</t>
+  </si>
+  <si>
+    <t>5.11.2021</t>
+  </si>
+  <si>
+    <t>6.11.2021</t>
+  </si>
+  <si>
+    <t>חיפה?</t>
+  </si>
+  <si>
+    <t>16.11.2021</t>
+  </si>
+  <si>
+    <t>20.11.2021</t>
+  </si>
+  <si>
+    <t>507456020, 522655783</t>
+  </si>
+  <si>
+    <t>חדרה</t>
+  </si>
+  <si>
+    <t>13.12.2021</t>
+  </si>
+  <si>
+    <t>29.12.2021</t>
+  </si>
+  <si>
+    <t>יקנעם</t>
+  </si>
+  <si>
+    <t>25.11.2021</t>
+  </si>
+  <si>
+    <t>11.12.2021</t>
+  </si>
+  <si>
+    <t>שתולה</t>
+  </si>
+  <si>
+    <t>טבעון</t>
+  </si>
+  <si>
+    <t>15.12.2021</t>
+  </si>
+  <si>
+    <t>שדה נחמיה</t>
+  </si>
+  <si>
+    <t>18.11.2021</t>
+  </si>
+  <si>
+    <t>בת ים</t>
+  </si>
+  <si>
+    <t>14.11.2021</t>
+  </si>
+  <si>
+    <t>02.12.2021</t>
+  </si>
+  <si>
+    <t>כמון</t>
+  </si>
+  <si>
+    <t>קרית שמונה</t>
+  </si>
+  <si>
+    <t>15.11.2021</t>
+  </si>
+  <si>
+    <t>נהריה</t>
+  </si>
+  <si>
+    <t>30.11.2021</t>
+  </si>
+  <si>
+    <t>05.12.201</t>
+  </si>
+  <si>
+    <t>שדה אילן</t>
+  </si>
+  <si>
+    <t>22.11.2021</t>
+  </si>
+  <si>
+    <t>29.11.2021</t>
+  </si>
+  <si>
+    <t>חולון</t>
+  </si>
+  <si>
+    <t>24.09.2021</t>
+  </si>
+  <si>
+    <t>31.01.2022</t>
+  </si>
+  <si>
+    <t>הררית</t>
+  </si>
+  <si>
+    <t>19.11.2021</t>
+  </si>
+  <si>
+    <t>אילון</t>
+  </si>
+  <si>
+    <t>533331723, 545688581</t>
+  </si>
+  <si>
+    <t>03.01.2022</t>
+  </si>
+  <si>
+    <t>23.12.2021</t>
+  </si>
+  <si>
+    <t>23.11.2021</t>
+  </si>
+  <si>
+    <t>דפנה</t>
+  </si>
+  <si>
+    <t>כפר אדמה</t>
+  </si>
+  <si>
+    <t>30.09.2021</t>
+  </si>
+  <si>
+    <t>01.03.2022</t>
+  </si>
+  <si>
+    <t>31.12.2021</t>
+  </si>
+  <si>
+    <t>12.11.2021</t>
+  </si>
+  <si>
+    <t>100 d</t>
+  </si>
+  <si>
+    <t>400 d</t>
+  </si>
+  <si>
+    <t>350 d</t>
+  </si>
+  <si>
+    <t>300 d</t>
+  </si>
+  <si>
+    <t>250 d</t>
+  </si>
+  <si>
+    <t>12000 m</t>
+  </si>
+  <si>
+    <t>3300 m</t>
+  </si>
+  <si>
+    <t>350, 490 d</t>
+  </si>
+  <si>
+    <t>150 d</t>
+  </si>
+  <si>
+    <t>1500, 2200 d</t>
+  </si>
+  <si>
+    <t>8750 m</t>
+  </si>
+  <si>
+    <t>5500 m</t>
+  </si>
+  <si>
+    <t>1400 11d</t>
+  </si>
+  <si>
+    <t>2100 m</t>
+  </si>
+  <si>
+    <t>1000 8d</t>
+  </si>
+  <si>
+    <t>2300 m</t>
+  </si>
+  <si>
+    <t>3600 m</t>
+  </si>
+  <si>
+    <t>1500 7d</t>
+  </si>
+  <si>
+    <t>300, 350 d</t>
+  </si>
+  <si>
+    <t>500 3d</t>
+  </si>
+  <si>
+    <t>3700 m</t>
+  </si>
+  <si>
+    <t>קרית טבעון</t>
+  </si>
+  <si>
+    <t>חיפה</t>
+  </si>
+  <si>
+    <t>3000 m</t>
+  </si>
+  <si>
+    <t>3800 m</t>
+  </si>
+  <si>
+    <t>1700 4d</t>
+  </si>
+  <si>
+    <t>06.12.2021</t>
+  </si>
+  <si>
+    <t>09.09.2021</t>
+  </si>
+  <si>
+    <t>12.12.2021</t>
+  </si>
+  <si>
+    <t>04.11.2021</t>
+  </si>
+  <si>
+    <t>06.11.2021</t>
+  </si>
+  <si>
+    <t>200 d</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2498,14 +2762,16 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2527,6 +2793,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2565,7 +2837,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -2583,13 +2855,35 @@
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="2" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="227581367215772297" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="-5935432621049393351" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="-5935432621049393351" xfId="2"/>
+    <cellStyle name="227581367215772297" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="50">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3319,21 +3613,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
     <col min="3" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3359,7 +3653,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -3372,8 +3666,8 @@
       <c r="D2" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="E2" s="4">
-        <v>100</v>
+      <c r="E2" s="4" t="s">
+        <v>478</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>423</v>
@@ -3382,10 +3676,10 @@
         <v>544747880</v>
       </c>
       <c r="H2" s="4">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -3411,7 +3705,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -3419,25 +3713,25 @@
         <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>10</v>
+        <v>424</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>11</v>
+        <v>425</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>13</v>
+        <v>426</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+      <c r="H4" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -3463,7 +3757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -3477,10 +3771,10 @@
         <v>11</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>12</v>
+        <v>479</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>13</v>
+        <v>427</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>14</v>
@@ -3489,7 +3783,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="112" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -3503,19 +3797,19 @@
         <v>11</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>12</v>
+        <v>480</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>14</v>
+        <v>427</v>
+      </c>
+      <c r="G7" s="4">
+        <v>539027197</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="210" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="224" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -3529,19 +3823,19 @@
         <v>11</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>12</v>
+        <v>481</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>13</v>
+        <v>428</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="240" x14ac:dyDescent="0.3">
+      <c r="H8" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="240" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -3549,25 +3843,25 @@
         <v>29</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>10</v>
+        <v>429</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>11</v>
+        <v>430</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>12</v>
+        <v>482</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>14</v>
+      <c r="G9" s="4">
+        <v>524465203</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="270" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="288" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -3584,16 +3878,16 @@
         <v>12</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>13</v>
+        <v>431</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>14</v>
+        <v>438</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="255" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
@@ -3607,19 +3901,19 @@
         <v>11</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>12</v>
+        <v>483</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="165" x14ac:dyDescent="0.3">
+        <v>426</v>
+      </c>
+      <c r="G11" s="4">
+        <v>505290072</v>
+      </c>
+      <c r="H11" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="176" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
@@ -3627,25 +3921,25 @@
         <v>35</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>10</v>
+        <v>433</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>11</v>
+        <v>434</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>14</v>
+        <v>432</v>
+      </c>
+      <c r="G12" s="4">
+        <v>503847930</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="255" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
@@ -3659,19 +3953,19 @@
         <v>11</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>12</v>
+        <v>484</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+        <v>435</v>
+      </c>
+      <c r="G13" s="4">
+        <v>535503661</v>
+      </c>
+      <c r="H13" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="409" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>38</v>
       </c>
@@ -3679,25 +3973,25 @@
         <v>39</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>10</v>
+        <v>436</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>11</v>
+        <v>437</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>12</v>
+        <v>485</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+        <v>426</v>
+      </c>
+      <c r="G14" s="4">
+        <v>544514010</v>
+      </c>
+      <c r="H14" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -3723,7 +4017,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="105" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="112" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>42</v>
       </c>
@@ -3731,16 +4025,16 @@
         <v>43</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>10</v>
+        <v>440</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>11</v>
+        <v>441</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>12</v>
+        <v>486</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>13</v>
+        <v>439</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>14</v>
@@ -3749,7 +4043,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
@@ -3766,7 +4060,7 @@
         <v>12</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>13</v>
+        <v>442</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>14</v>
@@ -3775,7 +4069,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="150" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="160" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>46</v>
       </c>
@@ -3783,29 +4077,29 @@
         <v>47</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>10</v>
+        <v>443</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>11</v>
+        <v>444</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>12</v>
+        <v>487</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+        <v>445</v>
+      </c>
+      <c r="G18" s="4">
+        <v>543286986</v>
+      </c>
+      <c r="H18" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -3827,7 +4121,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="150" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="160" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>50</v>
       </c>
@@ -3844,16 +4138,16 @@
         <v>12</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="195" x14ac:dyDescent="0.3">
+        <v>446</v>
+      </c>
+      <c r="G20" s="4">
+        <v>555613650</v>
+      </c>
+      <c r="H20" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="192" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
@@ -3861,25 +4155,25 @@
         <v>53</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>10</v>
+        <v>447</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>12</v>
+        <v>488</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>13</v>
+        <v>426</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H21" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+      <c r="H21" s="4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>54</v>
       </c>
@@ -3887,16 +4181,16 @@
         <v>55</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>10</v>
+        <v>449</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>11</v>
+        <v>437</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>12</v>
+        <v>487</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>13</v>
+        <v>448</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>14</v>
@@ -3905,7 +4199,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="180" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="192" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>56</v>
       </c>
@@ -3922,16 +4216,16 @@
         <v>12</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>13</v>
+        <v>450</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="240" x14ac:dyDescent="0.3">
+      <c r="H23" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="256" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>58</v>
       </c>
@@ -3945,19 +4239,19 @@
         <v>11</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>12</v>
+        <v>489</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+        <v>426</v>
+      </c>
+      <c r="G24" s="4">
+        <v>505290072</v>
+      </c>
+      <c r="H24" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>60</v>
       </c>
@@ -3965,25 +4259,25 @@
         <v>61</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>10</v>
+        <v>451</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>11</v>
+        <v>443</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>12</v>
+        <v>490</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>13</v>
+        <v>426</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H25" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+      <c r="H25" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>62</v>
       </c>
@@ -3991,25 +4285,25 @@
         <v>63</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>10</v>
+        <v>443</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>11</v>
+        <v>452</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>13</v>
+        <v>426</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H26" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+      <c r="H26" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>64</v>
       </c>
@@ -4026,16 +4320,16 @@
         <v>12</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>14</v>
+        <v>453</v>
+      </c>
+      <c r="G27" s="4">
+        <v>537295478</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>66</v>
       </c>
@@ -4052,16 +4346,16 @@
         <v>12</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>14</v>
+        <v>454</v>
+      </c>
+      <c r="G28" s="4">
+        <v>534301118</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>68</v>
       </c>
@@ -4069,25 +4363,25 @@
         <v>69</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>10</v>
+        <v>455</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>11</v>
+        <v>447</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>13</v>
+        <v>423</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+      <c r="H29" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>70</v>
       </c>
@@ -4095,16 +4389,16 @@
         <v>71</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>10</v>
+        <v>421</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>11</v>
+        <v>422</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>13</v>
+        <v>456</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>14</v>
@@ -4113,7 +4407,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="409" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>72</v>
       </c>
@@ -4124,22 +4418,22 @@
         <v>10</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>11</v>
+        <v>455</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>13</v>
+        <v>426</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H31" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+      <c r="H31" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>74</v>
       </c>
@@ -4153,7 +4447,7 @@
         <v>11</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>12</v>
+        <v>491</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>13</v>
@@ -4161,11 +4455,11 @@
       <c r="G32" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H32" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+      <c r="H32" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>76</v>
       </c>
@@ -4173,25 +4467,25 @@
         <v>77</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>10</v>
+        <v>457</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>11</v>
+        <v>458</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>14</v>
+        <v>459</v>
+      </c>
+      <c r="G33" s="4">
+        <v>528316179</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>78</v>
       </c>
@@ -4199,25 +4493,25 @@
         <v>79</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>10</v>
+        <v>460</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>11</v>
+        <v>461</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>12</v>
+        <v>492</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>13</v>
+        <v>462</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H34" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="180" x14ac:dyDescent="0.3">
+      <c r="H34" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="192" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>80</v>
       </c>
@@ -4231,19 +4525,19 @@
         <v>11</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>12</v>
+        <v>493</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>13</v>
+        <v>435</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H35" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="240" x14ac:dyDescent="0.3">
+      <c r="H35" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="256" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>82</v>
       </c>
@@ -4257,19 +4551,19 @@
         <v>11</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>12</v>
+        <v>489</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+        <v>426</v>
+      </c>
+      <c r="G36" s="4">
+        <v>505290072</v>
+      </c>
+      <c r="H36" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>84</v>
       </c>
@@ -4295,7 +4589,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>86</v>
       </c>
@@ -4303,25 +4597,25 @@
         <v>87</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>10</v>
+        <v>463</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>11</v>
+        <v>464</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>13</v>
+        <v>426</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H38" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="135" x14ac:dyDescent="0.3">
+      <c r="H38" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>88</v>
       </c>
@@ -4338,16 +4632,16 @@
         <v>12</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="105" x14ac:dyDescent="0.3">
+        <v>465</v>
+      </c>
+      <c r="G39" s="4">
+        <v>58448876</v>
+      </c>
+      <c r="H39" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="112" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>90</v>
       </c>
@@ -4355,25 +4649,25 @@
         <v>91</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>10</v>
+        <v>455</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>11</v>
+        <v>466</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>12</v>
+        <v>486</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>13</v>
+        <v>426</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H40" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="H40" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>92</v>
       </c>
@@ -4399,11 +4693,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -4425,7 +4719,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>94</v>
       </c>
@@ -4442,7 +4736,7 @@
         <v>12</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>13</v>
+        <v>467</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>14</v>
@@ -4451,7 +4745,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="195" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="208" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>96</v>
       </c>
@@ -4465,19 +4759,19 @@
         <v>11</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>12</v>
+        <v>494</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>13</v>
+        <v>435</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>14</v>
+        <v>468</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="75" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>98</v>
       </c>
@@ -4485,25 +4779,25 @@
         <v>99</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>10</v>
+        <v>470</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>11</v>
+        <v>469</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>12</v>
+        <v>495</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>13</v>
+        <v>427</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H45" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+      <c r="H45" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>100</v>
       </c>
@@ -4511,10 +4805,10 @@
         <v>101</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>10</v>
+        <v>471</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>11</v>
+        <v>457</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>12</v>
@@ -4529,7 +4823,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>102</v>
       </c>
@@ -4546,16 +4840,16 @@
         <v>12</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>13</v>
+        <v>472</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H47" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+      <c r="H47" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>104</v>
       </c>
@@ -4572,7 +4866,7 @@
         <v>12</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>13</v>
+        <v>442</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>14</v>
@@ -4581,7 +4875,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="195" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="208" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>105</v>
       </c>
@@ -4595,10 +4889,10 @@
         <v>11</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>12</v>
+        <v>496</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>13</v>
+        <v>473</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>14</v>
@@ -4607,7 +4901,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>107</v>
       </c>
@@ -4615,16 +4909,16 @@
         <v>108</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>10</v>
+        <v>429</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>11</v>
+        <v>430</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>12</v>
+        <v>497</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>13</v>
+        <v>427</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>14</v>
@@ -4633,7 +4927,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="75" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>109</v>
       </c>
@@ -4641,25 +4935,25 @@
         <v>110</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>10</v>
+        <v>474</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>11</v>
+        <v>475</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>13</v>
+        <v>426</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H51" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="H51" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>111</v>
       </c>
@@ -4685,7 +4979,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>113</v>
       </c>
@@ -4704,14 +4998,14 @@
       <c r="F53" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G53" s="4" t="s">
-        <v>14</v>
+      <c r="G53" s="4">
+        <v>523777810</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>115</v>
       </c>
@@ -4719,16 +5013,16 @@
         <v>116</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>10</v>
+        <v>476</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>11</v>
+        <v>425</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>12</v>
+        <v>498</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>13</v>
+        <v>423</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>14</v>
@@ -4737,7 +5031,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="285" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="304" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>117</v>
       </c>
@@ -4751,19 +5045,19 @@
         <v>11</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>12</v>
+        <v>483</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H55" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+        <v>423</v>
+      </c>
+      <c r="G55" s="4">
+        <v>505290072</v>
+      </c>
+      <c r="H55" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>119</v>
       </c>
@@ -4789,7 +5083,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>121</v>
       </c>
@@ -4815,7 +5109,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>123</v>
       </c>
@@ -4823,25 +5117,25 @@
         <v>124</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>10</v>
+        <v>477</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>11</v>
+        <v>422</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>14</v>
+        <v>427</v>
+      </c>
+      <c r="G58" s="4">
+        <v>543187550</v>
       </c>
       <c r="H58" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="150" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" ht="160" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>125</v>
       </c>
@@ -4858,16 +5152,16 @@
         <v>12</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G59" s="4" t="s">
-        <v>14</v>
+        <v>499</v>
+      </c>
+      <c r="G59" s="4">
+        <v>545510966</v>
       </c>
       <c r="H59" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="150" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>127</v>
       </c>
@@ -4884,16 +5178,16 @@
         <v>12</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>14</v>
+        <v>500</v>
+      </c>
+      <c r="G60" s="4">
+        <v>503200148</v>
       </c>
       <c r="H60" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="120" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" ht="128" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>129</v>
       </c>
@@ -4907,19 +5201,19 @@
         <v>11</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>12</v>
+        <v>501</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>14</v>
+        <v>426</v>
+      </c>
+      <c r="G61" s="4">
+        <v>546816048</v>
       </c>
       <c r="H61" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="225" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" ht="240" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>131</v>
       </c>
@@ -4933,19 +5227,19 @@
         <v>11</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>12</v>
+        <v>502</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H62" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="195" x14ac:dyDescent="0.3">
+        <v>426</v>
+      </c>
+      <c r="G62" s="4">
+        <v>505290072</v>
+      </c>
+      <c r="H62" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="208" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>133</v>
       </c>
@@ -4953,25 +5247,25 @@
         <v>134</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>10</v>
+        <v>452</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>11</v>
+        <v>504</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>12</v>
+        <v>503</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H63" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+        <v>431</v>
+      </c>
+      <c r="G63" s="4">
+        <v>502290056</v>
+      </c>
+      <c r="H63" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>135</v>
       </c>
@@ -4979,25 +5273,25 @@
         <v>136</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>10</v>
+        <v>505</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>11</v>
+        <v>464</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>13</v>
+        <v>426</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H64" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+      <c r="H64" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>137</v>
       </c>
@@ -5005,25 +5299,25 @@
         <v>138</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>10</v>
+        <v>429</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>11</v>
+        <v>506</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>13</v>
+        <v>423</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H65" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="285" x14ac:dyDescent="0.3">
+      <c r="H65" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="304" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>139</v>
       </c>
@@ -5031,25 +5325,25 @@
         <v>140</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>10</v>
+        <v>507</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>11</v>
+        <v>508</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>12</v>
+        <v>509</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>13</v>
+        <v>431</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H66" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="120" x14ac:dyDescent="0.3">
+      <c r="H66" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="128" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>141</v>
       </c>
@@ -5063,19 +5357,19 @@
         <v>11</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>12</v>
+        <v>501</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G67" s="4" t="s">
-        <v>14</v>
+        <v>426</v>
+      </c>
+      <c r="G67" s="4">
+        <v>546816048</v>
       </c>
       <c r="H67" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="135" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>142</v>
       </c>
@@ -5083,25 +5377,25 @@
         <v>143</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>10</v>
+        <v>460</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>11</v>
+        <v>444</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G68" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H68" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="120" x14ac:dyDescent="0.3">
+        <v>426</v>
+      </c>
+      <c r="G68" s="4">
+        <v>50555301</v>
+      </c>
+      <c r="H68" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="128" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>144</v>
       </c>
@@ -5123,11 +5417,11 @@
       <c r="G69" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H69" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="H69" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>146</v>
       </c>
@@ -5153,7 +5447,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>148</v>
       </c>
@@ -5179,7 +5473,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="165" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="160" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>150</v>
       </c>
@@ -5205,7 +5499,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="210" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="224" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>152</v>
       </c>
@@ -5231,7 +5525,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="165" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" ht="176" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>154</v>
       </c>
@@ -5257,7 +5551,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="409" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>156</v>
       </c>
@@ -5283,7 +5577,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="75" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>158</v>
       </c>
@@ -5309,7 +5603,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="105" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="112" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>160</v>
       </c>
@@ -5335,7 +5629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="315" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="304" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>162</v>
       </c>
@@ -5361,7 +5655,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>164</v>
       </c>
@@ -5387,7 +5681,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>166</v>
       </c>
@@ -5413,7 +5707,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>168</v>
       </c>
@@ -5439,7 +5733,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>170</v>
       </c>
@@ -5465,7 +5759,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>172</v>
       </c>
@@ -5491,7 +5785,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="210" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" ht="224" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>174</v>
       </c>
@@ -5517,7 +5811,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="210" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" ht="224" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>176</v>
       </c>
@@ -5543,7 +5837,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>178</v>
       </c>
@@ -5569,7 +5863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="195" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" ht="208" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>180</v>
       </c>
@@ -5595,7 +5889,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>182</v>
       </c>
@@ -5621,7 +5915,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="210" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" ht="224" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>184</v>
       </c>
@@ -5647,7 +5941,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>186</v>
       </c>
@@ -5673,7 +5967,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>188</v>
       </c>
@@ -5699,7 +5993,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>190</v>
       </c>
@@ -5725,7 +6019,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>192</v>
       </c>
@@ -5751,7 +6045,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="105" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" ht="112" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>194</v>
       </c>
@@ -5777,7 +6071,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="165" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" ht="176" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>196</v>
       </c>
@@ -5803,7 +6097,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="150" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" ht="112" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>198</v>
       </c>
@@ -5829,7 +6123,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="165" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" ht="176" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>200</v>
       </c>
@@ -5855,7 +6149,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>202</v>
       </c>
@@ -5881,7 +6175,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="375" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" ht="400" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>204</v>
       </c>
@@ -5907,7 +6201,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>206</v>
       </c>
@@ -5933,7 +6227,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="75" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>208</v>
       </c>
@@ -5961,63 +6255,73 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C101">
-    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="start_date">
+    <cfRule type="containsText" dxfId="49" priority="3" operator="containsText" text="start_date">
       <formula>NOT(ISERROR(SEARCH("start_date",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D101">
-    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="end_date">
+  <conditionalFormatting sqref="D2:D44 D46:D101">
+    <cfRule type="containsText" dxfId="48" priority="4" operator="containsText" text="end_date">
       <formula>NOT(ISERROR(SEARCH("end_date",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E101">
-    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="price">
+    <cfRule type="containsText" dxfId="47" priority="5" operator="containsText" text="price">
       <formula>NOT(ISERROR(SEARCH("price",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F101">
-    <cfRule type="containsText" dxfId="44" priority="4" operator="containsText" text="location">
+    <cfRule type="containsText" dxfId="46" priority="6" operator="containsText" text="location">
       <formula>NOT(ISERROR(SEARCH("location",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G101">
-    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="phone_number">
+    <cfRule type="containsText" dxfId="45" priority="7" operator="containsText" text="phone_number">
       <formula>NOT(ISERROR(SEARCH("phone_number",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H101">
-    <cfRule type="containsText" dxfId="42" priority="6" operator="containsText" text="rooms">
+    <cfRule type="containsText" dxfId="44" priority="8" operator="containsText" text="rooms">
       <formula>NOT(ISERROR(SEARCH("rooms",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C101">
-    <cfRule type="expression" dxfId="41" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="9" stopIfTrue="1">
       <formula>ISBLANK(C1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D101">
-    <cfRule type="expression" dxfId="40" priority="8" stopIfTrue="1">
+  <conditionalFormatting sqref="D1:D44 D46:D101">
+    <cfRule type="expression" dxfId="42" priority="10" stopIfTrue="1">
       <formula>ISBLANK(D1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E101">
-    <cfRule type="expression" dxfId="39" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="11" stopIfTrue="1">
       <formula>ISBLANK(E1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F101">
-    <cfRule type="expression" dxfId="38" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="12" stopIfTrue="1">
       <formula>ISBLANK(F1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G101">
-    <cfRule type="expression" dxfId="37" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="13" stopIfTrue="1">
       <formula>ISBLANK(G1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H101">
-    <cfRule type="expression" dxfId="36" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="14" stopIfTrue="1">
       <formula>ISBLANK(H1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="start_date">
+      <formula>NOT(ISERROR(SEARCH("start_date",D45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+      <formula>ISBLANK(D45)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6025,19 +6329,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
     <col min="3" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6063,7 +6367,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>210</v>
       </c>
@@ -6089,7 +6393,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>212</v>
       </c>
@@ -6115,7 +6419,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="165" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="176" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>214</v>
       </c>
@@ -6141,7 +6445,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>216</v>
       </c>
@@ -6167,7 +6471,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="285" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="288" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>218</v>
       </c>
@@ -6193,7 +6497,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>220</v>
       </c>
@@ -6219,7 +6523,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="112" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>222</v>
       </c>
@@ -6245,7 +6549,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="120" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="112" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>224</v>
       </c>
@@ -6271,7 +6575,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="285" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>226</v>
       </c>
@@ -6297,7 +6601,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="270" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>228</v>
       </c>
@@ -6323,7 +6627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="255" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>230</v>
       </c>
@@ -6349,7 +6653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>232</v>
       </c>
@@ -6375,7 +6679,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="409" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>234</v>
       </c>
@@ -6401,7 +6705,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="210" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="224" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>236</v>
       </c>
@@ -6427,7 +6731,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>237</v>
       </c>
@@ -6453,7 +6757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="150" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="112" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>239</v>
       </c>
@@ -6479,7 +6783,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>240</v>
       </c>
@@ -6505,7 +6809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="135" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="128" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>242</v>
       </c>
@@ -6531,7 +6835,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="409" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>244</v>
       </c>
@@ -6557,7 +6861,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>245</v>
       </c>
@@ -6583,7 +6887,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>247</v>
       </c>
@@ -6609,7 +6913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="270" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="288" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>249</v>
       </c>
@@ -6635,7 +6939,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>251</v>
       </c>
@@ -6661,7 +6965,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="135" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>253</v>
       </c>
@@ -6687,7 +6991,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>255</v>
       </c>
@@ -6713,7 +7017,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="255" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>257</v>
       </c>
@@ -6739,7 +7043,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="240" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="256" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>259</v>
       </c>
@@ -6765,7 +7069,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>261</v>
       </c>
@@ -6791,7 +7095,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>263</v>
       </c>
@@ -6817,7 +7121,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="240" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="256" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>264</v>
       </c>
@@ -6843,7 +7147,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>266</v>
       </c>
@@ -6869,7 +7173,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>268</v>
       </c>
@@ -6895,7 +7199,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="105" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="112" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>269</v>
       </c>
@@ -6921,7 +7225,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>271</v>
       </c>
@@ -6947,7 +7251,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>273</v>
       </c>
@@ -6973,7 +7277,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="120" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="128" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>274</v>
       </c>
@@ -6999,7 +7303,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="210" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="224" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>276</v>
       </c>
@@ -7025,7 +7329,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>278</v>
       </c>
@@ -7051,7 +7355,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="180" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="192" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>280</v>
       </c>
@@ -7077,7 +7381,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>282</v>
       </c>
@@ -7103,7 +7407,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>284</v>
       </c>
@@ -7129,7 +7433,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="195" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="208" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>286</v>
       </c>
@@ -7155,7 +7459,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="105" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>288</v>
       </c>
@@ -7181,7 +7485,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="105" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>290</v>
       </c>
@@ -7207,7 +7511,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="120" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="128" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>292</v>
       </c>
@@ -7233,7 +7537,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="105" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="112" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>294</v>
       </c>
@@ -7259,7 +7563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="285" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="304" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>296</v>
       </c>
@@ -7285,7 +7589,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="255" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>298</v>
       </c>
@@ -7311,7 +7615,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>300</v>
       </c>
@@ -7337,7 +7641,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>301</v>
       </c>
@@ -7363,7 +7667,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="240" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" ht="240" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>303</v>
       </c>
@@ -7389,7 +7693,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>305</v>
       </c>
@@ -7415,7 +7719,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="75" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>307</v>
       </c>
@@ -7441,7 +7745,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="120" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="128" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>309</v>
       </c>
@@ -7467,7 +7771,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>311</v>
       </c>
@@ -7493,7 +7797,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="135" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>313</v>
       </c>
@@ -7519,7 +7823,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="135" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>315</v>
       </c>
@@ -7545,7 +7849,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="330" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" ht="320" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>317</v>
       </c>
@@ -7571,7 +7875,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>319</v>
       </c>
@@ -7597,7 +7901,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>321</v>
       </c>
@@ -7621,7 +7925,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="195" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" ht="208" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>322</v>
       </c>
@@ -7647,7 +7951,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="135" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>324</v>
       </c>
@@ -7673,7 +7977,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>326</v>
       </c>
@@ -7697,7 +8001,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="285" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>327</v>
       </c>
@@ -7723,7 +8027,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>329</v>
       </c>
@@ -7749,7 +8053,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="180" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="192" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>331</v>
       </c>
@@ -7775,7 +8079,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>333</v>
       </c>
@@ -7801,7 +8105,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>335</v>
       </c>
@@ -7827,7 +8131,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>337</v>
       </c>
@@ -7853,7 +8157,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>338</v>
       </c>
@@ -7879,7 +8183,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>340</v>
       </c>
@@ -7905,7 +8209,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="390" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="409" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>342</v>
       </c>
@@ -7931,7 +8235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="75" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>344</v>
       </c>
@@ -7957,7 +8261,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>346</v>
       </c>
@@ -7983,7 +8287,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="180" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" ht="192" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>348</v>
       </c>
@@ -8009,7 +8313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>350</v>
       </c>
@@ -8033,7 +8337,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="180" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="192" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>351</v>
       </c>
@@ -8059,7 +8363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>353</v>
       </c>
@@ -8085,7 +8389,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>355</v>
       </c>
@@ -8111,7 +8415,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>357</v>
       </c>
@@ -8137,7 +8441,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>359</v>
       </c>
@@ -8163,7 +8467,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="75" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>360</v>
       </c>
@@ -8189,7 +8493,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>362</v>
       </c>
@@ -8215,7 +8519,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>364</v>
       </c>
@@ -8241,7 +8545,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="75" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>366</v>
       </c>
@@ -8267,7 +8571,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="150" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" ht="160" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>368</v>
       </c>
@@ -8293,7 +8597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="165" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" ht="160" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>370</v>
       </c>
@@ -8319,7 +8623,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="75" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>372</v>
       </c>
@@ -8345,7 +8649,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>374</v>
       </c>
@@ -8371,7 +8675,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>375</v>
       </c>
@@ -8397,7 +8701,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="345" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" ht="352" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>377</v>
       </c>
@@ -8423,7 +8727,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>379</v>
       </c>
@@ -8449,7 +8753,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="135" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>381</v>
       </c>
@@ -8475,7 +8779,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>383</v>
       </c>
@@ -8501,7 +8805,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>385</v>
       </c>
@@ -8527,7 +8831,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>387</v>
       </c>
@@ -8553,7 +8857,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>389</v>
       </c>
@@ -8579,7 +8883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>391</v>
       </c>
@@ -8605,7 +8909,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>393</v>
       </c>
@@ -8631,7 +8935,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>395</v>
       </c>
@@ -8659,62 +8963,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C101">
-    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="start_date">
+    <cfRule type="containsText" dxfId="37" priority="1" operator="containsText" text="start_date">
       <formula>NOT(ISERROR(SEARCH("start_date",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D101">
-    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="end_date">
+    <cfRule type="containsText" dxfId="36" priority="2" operator="containsText" text="end_date">
       <formula>NOT(ISERROR(SEARCH("end_date",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E101">
-    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="price">
+    <cfRule type="containsText" dxfId="35" priority="3" operator="containsText" text="price">
       <formula>NOT(ISERROR(SEARCH("price",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F101">
-    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="location">
+    <cfRule type="containsText" dxfId="34" priority="4" operator="containsText" text="location">
       <formula>NOT(ISERROR(SEARCH("location",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G101">
-    <cfRule type="containsText" dxfId="31" priority="5" operator="containsText" text="phone_number">
+    <cfRule type="containsText" dxfId="33" priority="5" operator="containsText" text="phone_number">
       <formula>NOT(ISERROR(SEARCH("phone_number",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H101">
-    <cfRule type="containsText" dxfId="30" priority="6" operator="containsText" text="rooms">
+    <cfRule type="containsText" dxfId="32" priority="6" operator="containsText" text="rooms">
       <formula>NOT(ISERROR(SEARCH("rooms",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C101">
-    <cfRule type="expression" dxfId="29" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="7" stopIfTrue="1">
       <formula>ISBLANK(C1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D101">
-    <cfRule type="expression" dxfId="28" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="8" stopIfTrue="1">
       <formula>ISBLANK(D1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E101">
-    <cfRule type="expression" dxfId="27" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="9" stopIfTrue="1">
       <formula>ISBLANK(E1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F101">
-    <cfRule type="expression" dxfId="26" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="10" stopIfTrue="1">
       <formula>ISBLANK(F1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G101">
-    <cfRule type="expression" dxfId="25" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="11" stopIfTrue="1">
       <formula>ISBLANK(G1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H101">
-    <cfRule type="expression" dxfId="24" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="12" stopIfTrue="1">
       <formula>ISBLANK(H1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8723,19 +9027,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
     <col min="3" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8761,7 +9065,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="105" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>397</v>
       </c>
@@ -8787,7 +9091,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="270" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>399</v>
       </c>
@@ -8813,7 +9117,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>401</v>
       </c>
@@ -8839,7 +9143,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="210" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="224" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>403</v>
       </c>
@@ -8865,7 +9169,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>405</v>
       </c>
@@ -8891,7 +9195,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="240" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="256" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>406</v>
       </c>
@@ -8917,7 +9221,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="150" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="160" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>407</v>
       </c>
@@ -8943,7 +9247,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="195" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="208" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>409</v>
       </c>
@@ -8969,7 +9273,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>411</v>
       </c>
@@ -8995,7 +9299,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="409" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>413</v>
       </c>
@@ -9021,7 +9325,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="240" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="256" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>415</v>
       </c>
@@ -9047,7 +9351,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>417</v>
       </c>
@@ -9073,7 +9377,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="240" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="256" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>419</v>
       </c>
@@ -9101,62 +9405,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C101">
-    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="start_date">
+    <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="start_date">
       <formula>NOT(ISERROR(SEARCH("start_date",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D101">
-    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="end_date">
+    <cfRule type="containsText" dxfId="24" priority="2" operator="containsText" text="end_date">
       <formula>NOT(ISERROR(SEARCH("end_date",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E101">
-    <cfRule type="containsText" dxfId="21" priority="3" operator="containsText" text="price">
+    <cfRule type="containsText" dxfId="23" priority="3" operator="containsText" text="price">
       <formula>NOT(ISERROR(SEARCH("price",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F101">
-    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="location">
+    <cfRule type="containsText" dxfId="22" priority="4" operator="containsText" text="location">
       <formula>NOT(ISERROR(SEARCH("location",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G101">
-    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="phone_number">
+    <cfRule type="containsText" dxfId="21" priority="5" operator="containsText" text="phone_number">
       <formula>NOT(ISERROR(SEARCH("phone_number",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H101">
-    <cfRule type="containsText" dxfId="18" priority="6" operator="containsText" text="rooms">
+    <cfRule type="containsText" dxfId="20" priority="6" operator="containsText" text="rooms">
       <formula>NOT(ISERROR(SEARCH("rooms",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C101">
-    <cfRule type="expression" dxfId="17" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="7" stopIfTrue="1">
       <formula>ISBLANK(C1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D101">
-    <cfRule type="expression" dxfId="16" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="8" stopIfTrue="1">
       <formula>ISBLANK(D1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E101">
-    <cfRule type="expression" dxfId="15" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="9" stopIfTrue="1">
       <formula>ISBLANK(E1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F101">
-    <cfRule type="expression" dxfId="14" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="10" stopIfTrue="1">
       <formula>ISBLANK(F1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G101">
-    <cfRule type="expression" dxfId="13" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="11" stopIfTrue="1">
       <formula>ISBLANK(G1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H101">
-    <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="12" stopIfTrue="1">
       <formula>ISBLANK(H1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9165,19 +9469,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
     <col min="3" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9205,62 +9509,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C101">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="start_date">
+    <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="start_date">
       <formula>NOT(ISERROR(SEARCH("start_date",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D101">
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="end_date">
+    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="end_date">
       <formula>NOT(ISERROR(SEARCH("end_date",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E101">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="price">
+    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="price">
       <formula>NOT(ISERROR(SEARCH("price",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F101">
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="location">
+    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="location">
       <formula>NOT(ISERROR(SEARCH("location",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G101">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="phone_number">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="phone_number">
       <formula>NOT(ISERROR(SEARCH("phone_number",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H101">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="rooms">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="rooms">
       <formula>NOT(ISERROR(SEARCH("rooms",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C101">
-    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
       <formula>ISBLANK(C1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D101">
-    <cfRule type="expression" dxfId="4" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
       <formula>ISBLANK(D1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E101">
-    <cfRule type="expression" dxfId="3" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="9" stopIfTrue="1">
       <formula>ISBLANK(E1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F101">
-    <cfRule type="expression" dxfId="2" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="10" stopIfTrue="1">
       <formula>ISBLANK(F1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G101">
-    <cfRule type="expression" dxfId="1" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="11" stopIfTrue="1">
       <formula>ISBLANK(G1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H101">
-    <cfRule type="expression" dxfId="0" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="12" stopIfTrue="1">
       <formula>ISBLANK(H1)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix todos from code review: 1. parse price correctly from tagging_utils.py 2. add streets to parse location in tel aviv and jerusalem 3. add whatapp class
</commit_message>
<xml_diff>
--- a/data_utils/data_for_tagging.xlsx
+++ b/data_utils/data_for_tagging.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eliyasegev/PycharmProjects/traveliz/data_utils/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Y\PycharmProjects\traveliz\data_utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9664FEE-574E-460F-B46E-012200F9CC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="facebook_posts_1" sheetId="1" r:id="rId1"/>
@@ -2589,9 +2590,6 @@
     <t>30.11.2021</t>
   </si>
   <si>
-    <t>05.12.201</t>
-  </si>
-  <si>
     <t>שדה אילן</t>
   </si>
   <si>
@@ -2670,15 +2668,9 @@
     <t>3300 m</t>
   </si>
   <si>
-    <t>350, 490 d</t>
-  </si>
-  <si>
     <t>150 d</t>
   </si>
   <si>
-    <t>1500, 2200 d</t>
-  </si>
-  <si>
     <t>8750 m</t>
   </si>
   <si>
@@ -2703,9 +2695,6 @@
     <t>1500 7d</t>
   </si>
   <si>
-    <t>300, 350 d</t>
-  </si>
-  <si>
     <t>500 3d</t>
   </si>
   <si>
@@ -2743,12 +2732,24 @@
   </si>
   <si>
     <t>200 d</t>
+  </si>
+  <si>
+    <t>1500 d, 2200 d</t>
+  </si>
+  <si>
+    <t>300 d, 350 d</t>
+  </si>
+  <si>
+    <t>350 d, 490 d</t>
+  </si>
+  <si>
+    <t>05.12.2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2861,29 +2862,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="-5935432621049393351" xfId="2"/>
-    <cellStyle name="227581367215772297" xfId="1"/>
+    <cellStyle name="227581367215772297" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="-5935432621049393351" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="50">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3195,6 +3178,24 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3613,21 +3614,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
     <col min="3" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3653,7 +3654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -3667,7 +3668,7 @@
         <v>422</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>423</v>
@@ -3679,7 +3680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -3705,7 +3706,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -3731,7 +3732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -3757,7 +3758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -3771,7 +3772,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>427</v>
@@ -3783,7 +3784,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -3797,7 +3798,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>427</v>
@@ -3809,7 +3810,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -3823,7 +3824,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>428</v>
@@ -3835,7 +3836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="240" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -3849,7 +3850,7 @@
         <v>430</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>13</v>
@@ -3861,7 +3862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="288" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="270" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -3887,7 +3888,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="255" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
@@ -3901,7 +3902,7 @@
         <v>11</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>426</v>
@@ -3913,7 +3914,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
@@ -3939,7 +3940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="255" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
@@ -3953,7 +3954,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>435</v>
@@ -3965,7 +3966,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>38</v>
       </c>
@@ -3979,7 +3980,7 @@
         <v>437</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>485</v>
+        <v>508</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>426</v>
@@ -3991,7 +3992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -4017,7 +4018,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>42</v>
       </c>
@@ -4031,7 +4032,7 @@
         <v>441</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>439</v>
@@ -4043,7 +4044,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
@@ -4069,7 +4070,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>46</v>
       </c>
@@ -4083,7 +4084,7 @@
         <v>444</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>487</v>
+        <v>506</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>445</v>
@@ -4095,7 +4096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>48</v>
       </c>
@@ -4121,7 +4122,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>50</v>
       </c>
@@ -4147,7 +4148,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
@@ -4161,7 +4162,7 @@
         <v>11</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>426</v>
@@ -4173,7 +4174,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>54</v>
       </c>
@@ -4187,7 +4188,7 @@
         <v>437</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>487</v>
+        <v>506</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>448</v>
@@ -4199,7 +4200,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="180" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>56</v>
       </c>
@@ -4225,7 +4226,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>58</v>
       </c>
@@ -4239,7 +4240,7 @@
         <v>11</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>426</v>
@@ -4251,7 +4252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>60</v>
       </c>
@@ -4265,7 +4266,7 @@
         <v>443</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>426</v>
@@ -4277,7 +4278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>62</v>
       </c>
@@ -4303,7 +4304,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>64</v>
       </c>
@@ -4329,7 +4330,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>66</v>
       </c>
@@ -4355,7 +4356,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>68</v>
       </c>
@@ -4381,7 +4382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>70</v>
       </c>
@@ -4407,7 +4408,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>72</v>
       </c>
@@ -4433,7 +4434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>74</v>
       </c>
@@ -4447,7 +4448,7 @@
         <v>11</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>13</v>
@@ -4459,7 +4460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>76</v>
       </c>
@@ -4470,13 +4471,13 @@
         <v>457</v>
       </c>
       <c r="D33" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>458</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>459</v>
       </c>
       <c r="G33" s="4">
         <v>528316179</v>
@@ -4485,7 +4486,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>78</v>
       </c>
@@ -4493,16 +4494,16 @@
         <v>79</v>
       </c>
       <c r="C34" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>460</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="E34" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>461</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>492</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>462</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>14</v>
@@ -4511,7 +4512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="180" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>80</v>
       </c>
@@ -4525,7 +4526,7 @@
         <v>11</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>435</v>
@@ -4537,7 +4538,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>82</v>
       </c>
@@ -4551,7 +4552,7 @@
         <v>11</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>426</v>
@@ -4563,7 +4564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>84</v>
       </c>
@@ -4589,7 +4590,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>86</v>
       </c>
@@ -4597,10 +4598,10 @@
         <v>87</v>
       </c>
       <c r="C38" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>463</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>464</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>12</v>
@@ -4615,7 +4616,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>88</v>
       </c>
@@ -4632,7 +4633,7 @@
         <v>12</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G39" s="4">
         <v>58448876</v>
@@ -4641,7 +4642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>90</v>
       </c>
@@ -4652,10 +4653,10 @@
         <v>455</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>426</v>
@@ -4667,7 +4668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>92</v>
       </c>
@@ -4693,7 +4694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>48</v>
       </c>
@@ -4719,7 +4720,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>94</v>
       </c>
@@ -4736,7 +4737,7 @@
         <v>12</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>14</v>
@@ -4745,7 +4746,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>96</v>
       </c>
@@ -4759,19 +4760,19 @@
         <v>11</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>435</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>98</v>
       </c>
@@ -4779,13 +4780,13 @@
         <v>99</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>427</v>
@@ -4797,7 +4798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>100</v>
       </c>
@@ -4805,7 +4806,7 @@
         <v>101</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>457</v>
@@ -4823,7 +4824,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>102</v>
       </c>
@@ -4840,7 +4841,7 @@
         <v>12</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>14</v>
@@ -4849,7 +4850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>104</v>
       </c>
@@ -4875,7 +4876,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>105</v>
       </c>
@@ -4889,10 +4890,10 @@
         <v>11</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>496</v>
+        <v>507</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>14</v>
@@ -4901,7 +4902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>107</v>
       </c>
@@ -4915,7 +4916,7 @@
         <v>430</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>427</v>
@@ -4927,7 +4928,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>109</v>
       </c>
@@ -4935,10 +4936,10 @@
         <v>110</v>
       </c>
       <c r="C51" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>474</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>475</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>12</v>
@@ -4953,7 +4954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>111</v>
       </c>
@@ -4979,7 +4980,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>113</v>
       </c>
@@ -5005,7 +5006,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>115</v>
       </c>
@@ -5013,13 +5014,13 @@
         <v>116</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>425</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="F54" s="4" t="s">
         <v>423</v>
@@ -5031,7 +5032,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="304" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" ht="285" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>117</v>
       </c>
@@ -5045,7 +5046,7 @@
         <v>11</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F55" s="4" t="s">
         <v>423</v>
@@ -5057,7 +5058,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>119</v>
       </c>
@@ -5083,7 +5084,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>121</v>
       </c>
@@ -5109,7 +5110,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>123</v>
       </c>
@@ -5117,7 +5118,7 @@
         <v>124</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>422</v>
@@ -5135,7 +5136,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>125</v>
       </c>
@@ -5152,7 +5153,7 @@
         <v>12</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="G59" s="4">
         <v>545510966</v>
@@ -5161,7 +5162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>127</v>
       </c>
@@ -5178,7 +5179,7 @@
         <v>12</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="G60" s="4">
         <v>503200148</v>
@@ -5187,7 +5188,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>129</v>
       </c>
@@ -5201,7 +5202,7 @@
         <v>11</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="F61" s="4" t="s">
         <v>426</v>
@@ -5213,7 +5214,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="240" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" ht="225" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>131</v>
       </c>
@@ -5227,7 +5228,7 @@
         <v>11</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="F62" s="4" t="s">
         <v>426</v>
@@ -5239,7 +5240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>133</v>
       </c>
@@ -5250,10 +5251,10 @@
         <v>452</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="F63" s="4" t="s">
         <v>431</v>
@@ -5265,7 +5266,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>135</v>
       </c>
@@ -5273,10 +5274,10 @@
         <v>136</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>12</v>
@@ -5291,7 +5292,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>137</v>
       </c>
@@ -5302,7 +5303,7 @@
         <v>429</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>12</v>
@@ -5317,7 +5318,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="304" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" ht="285" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>139</v>
       </c>
@@ -5325,13 +5326,13 @@
         <v>140</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>431</v>
@@ -5343,7 +5344,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>141</v>
       </c>
@@ -5357,7 +5358,7 @@
         <v>11</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="F67" s="4" t="s">
         <v>426</v>
@@ -5369,7 +5370,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>142</v>
       </c>
@@ -5377,7 +5378,7 @@
         <v>143</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>444</v>
@@ -5395,7 +5396,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>144</v>
       </c>
@@ -5421,7 +5422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>146</v>
       </c>
@@ -5447,7 +5448,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>148</v>
       </c>
@@ -5473,7 +5474,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>150</v>
       </c>
@@ -5499,7 +5500,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>152</v>
       </c>
@@ -5525,7 +5526,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>154</v>
       </c>
@@ -5551,7 +5552,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>156</v>
       </c>
@@ -5577,7 +5578,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>158</v>
       </c>
@@ -5603,7 +5604,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>160</v>
       </c>
@@ -5629,7 +5630,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="304" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" ht="315" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>162</v>
       </c>
@@ -5655,7 +5656,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>164</v>
       </c>
@@ -5681,7 +5682,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>166</v>
       </c>
@@ -5707,7 +5708,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>168</v>
       </c>
@@ -5733,7 +5734,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>170</v>
       </c>
@@ -5759,7 +5760,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>172</v>
       </c>
@@ -5785,7 +5786,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>174</v>
       </c>
@@ -5811,7 +5812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>176</v>
       </c>
@@ -5837,7 +5838,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>178</v>
       </c>
@@ -5863,7 +5864,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>180</v>
       </c>
@@ -5889,7 +5890,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>182</v>
       </c>
@@ -5915,7 +5916,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>184</v>
       </c>
@@ -5941,7 +5942,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>186</v>
       </c>
@@ -5967,7 +5968,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>188</v>
       </c>
@@ -5993,7 +5994,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>190</v>
       </c>
@@ -6019,7 +6020,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>192</v>
       </c>
@@ -6045,7 +6046,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>194</v>
       </c>
@@ -6071,7 +6072,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>196</v>
       </c>
@@ -6097,7 +6098,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>198</v>
       </c>
@@ -6123,7 +6124,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>200</v>
       </c>
@@ -6149,7 +6150,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>202</v>
       </c>
@@ -6175,7 +6176,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="400" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" ht="375" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>204</v>
       </c>
@@ -6201,7 +6202,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>206</v>
       </c>
@@ -6227,7 +6228,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>208</v>
       </c>
@@ -6315,12 +6316,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="start_date">
+    <cfRule type="containsText" dxfId="37" priority="1" operator="containsText" text="start_date">
       <formula>NOT(ISERROR(SEARCH("start_date",D45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="2" stopIfTrue="1">
       <formula>ISBLANK(D45)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6329,19 +6330,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
     <col min="3" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6367,7 +6368,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>210</v>
       </c>
@@ -6393,7 +6394,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>212</v>
       </c>
@@ -6419,7 +6420,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>214</v>
       </c>
@@ -6445,7 +6446,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>216</v>
       </c>
@@ -6471,7 +6472,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="288" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="285" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>218</v>
       </c>
@@ -6497,7 +6498,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>220</v>
       </c>
@@ -6523,7 +6524,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>222</v>
       </c>
@@ -6549,7 +6550,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>224</v>
       </c>
@@ -6575,7 +6576,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="285" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>226</v>
       </c>
@@ -6601,7 +6602,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="270" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>228</v>
       </c>
@@ -6627,7 +6628,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="255" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>230</v>
       </c>
@@ -6653,7 +6654,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>232</v>
       </c>
@@ -6679,7 +6680,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>234</v>
       </c>
@@ -6705,7 +6706,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>236</v>
       </c>
@@ -6731,7 +6732,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>237</v>
       </c>
@@ -6757,7 +6758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>239</v>
       </c>
@@ -6783,7 +6784,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>240</v>
       </c>
@@ -6809,7 +6810,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>242</v>
       </c>
@@ -6835,7 +6836,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>244</v>
       </c>
@@ -6861,7 +6862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>245</v>
       </c>
@@ -6887,7 +6888,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>247</v>
       </c>
@@ -6913,7 +6914,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="288" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="270" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>249</v>
       </c>
@@ -6939,7 +6940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>251</v>
       </c>
@@ -6965,7 +6966,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>253</v>
       </c>
@@ -6991,7 +6992,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>255</v>
       </c>
@@ -7017,7 +7018,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="255" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>257</v>
       </c>
@@ -7043,7 +7044,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>259</v>
       </c>
@@ -7069,7 +7070,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>261</v>
       </c>
@@ -7095,7 +7096,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>263</v>
       </c>
@@ -7121,7 +7122,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>264</v>
       </c>
@@ -7147,7 +7148,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>266</v>
       </c>
@@ -7173,7 +7174,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>268</v>
       </c>
@@ -7199,7 +7200,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>269</v>
       </c>
@@ -7225,7 +7226,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>271</v>
       </c>
@@ -7251,7 +7252,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>273</v>
       </c>
@@ -7277,7 +7278,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>274</v>
       </c>
@@ -7303,7 +7304,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>276</v>
       </c>
@@ -7329,7 +7330,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>278</v>
       </c>
@@ -7355,7 +7356,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" ht="180" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>280</v>
       </c>
@@ -7381,7 +7382,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>282</v>
       </c>
@@ -7407,7 +7408,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>284</v>
       </c>
@@ -7433,7 +7434,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>286</v>
       </c>
@@ -7459,7 +7460,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>288</v>
       </c>
@@ -7485,7 +7486,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>290</v>
       </c>
@@ -7511,7 +7512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>292</v>
       </c>
@@ -7537,7 +7538,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>294</v>
       </c>
@@ -7563,7 +7564,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="304" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" ht="285" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>296</v>
       </c>
@@ -7589,7 +7590,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" ht="255" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>298</v>
       </c>
@@ -7615,7 +7616,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>300</v>
       </c>
@@ -7641,7 +7642,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>301</v>
       </c>
@@ -7667,7 +7668,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="240" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>303</v>
       </c>
@@ -7693,7 +7694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>305</v>
       </c>
@@ -7719,7 +7720,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>307</v>
       </c>
@@ -7745,7 +7746,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>309</v>
       </c>
@@ -7771,7 +7772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>311</v>
       </c>
@@ -7797,7 +7798,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>313</v>
       </c>
@@ -7823,7 +7824,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>315</v>
       </c>
@@ -7849,7 +7850,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="320" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" ht="330" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>317</v>
       </c>
@@ -7875,7 +7876,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>319</v>
       </c>
@@ -7901,7 +7902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>321</v>
       </c>
@@ -7925,7 +7926,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>322</v>
       </c>
@@ -7951,7 +7952,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>324</v>
       </c>
@@ -7977,7 +7978,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>326</v>
       </c>
@@ -8001,7 +8002,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" ht="285" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>327</v>
       </c>
@@ -8027,7 +8028,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>329</v>
       </c>
@@ -8053,7 +8054,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" ht="180" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>331</v>
       </c>
@@ -8079,7 +8080,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>333</v>
       </c>
@@ -8105,7 +8106,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>335</v>
       </c>
@@ -8131,7 +8132,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>337</v>
       </c>
@@ -8157,7 +8158,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>338</v>
       </c>
@@ -8183,7 +8184,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>340</v>
       </c>
@@ -8209,7 +8210,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" ht="390" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>342</v>
       </c>
@@ -8235,7 +8236,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>344</v>
       </c>
@@ -8261,7 +8262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>346</v>
       </c>
@@ -8287,7 +8288,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" ht="180" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>348</v>
       </c>
@@ -8313,7 +8314,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>350</v>
       </c>
@@ -8337,7 +8338,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" ht="180" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>351</v>
       </c>
@@ -8363,7 +8364,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>353</v>
       </c>
@@ -8389,7 +8390,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>355</v>
       </c>
@@ -8415,7 +8416,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>357</v>
       </c>
@@ -8441,7 +8442,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>359</v>
       </c>
@@ -8467,7 +8468,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>360</v>
       </c>
@@ -8493,7 +8494,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>362</v>
       </c>
@@ -8519,7 +8520,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>364</v>
       </c>
@@ -8545,7 +8546,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>366</v>
       </c>
@@ -8571,7 +8572,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>368</v>
       </c>
@@ -8597,7 +8598,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>370</v>
       </c>
@@ -8623,7 +8624,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>372</v>
       </c>
@@ -8649,7 +8650,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>374</v>
       </c>
@@ -8675,7 +8676,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>375</v>
       </c>
@@ -8701,7 +8702,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="352" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" ht="345" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>377</v>
       </c>
@@ -8727,7 +8728,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>379</v>
       </c>
@@ -8753,7 +8754,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>381</v>
       </c>
@@ -8779,7 +8780,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>383</v>
       </c>
@@ -8805,7 +8806,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>385</v>
       </c>
@@ -8831,7 +8832,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>387</v>
       </c>
@@ -8857,7 +8858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>389</v>
       </c>
@@ -8883,7 +8884,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>391</v>
       </c>
@@ -8909,7 +8910,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>393</v>
       </c>
@@ -8935,7 +8936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>395</v>
       </c>
@@ -8963,62 +8964,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C101">
-    <cfRule type="containsText" dxfId="37" priority="1" operator="containsText" text="start_date">
+    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="start_date">
       <formula>NOT(ISERROR(SEARCH("start_date",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D101">
-    <cfRule type="containsText" dxfId="36" priority="2" operator="containsText" text="end_date">
+    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="end_date">
       <formula>NOT(ISERROR(SEARCH("end_date",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E101">
-    <cfRule type="containsText" dxfId="35" priority="3" operator="containsText" text="price">
+    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="price">
       <formula>NOT(ISERROR(SEARCH("price",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F101">
-    <cfRule type="containsText" dxfId="34" priority="4" operator="containsText" text="location">
+    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="location">
       <formula>NOT(ISERROR(SEARCH("location",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G101">
-    <cfRule type="containsText" dxfId="33" priority="5" operator="containsText" text="phone_number">
+    <cfRule type="containsText" dxfId="31" priority="5" operator="containsText" text="phone_number">
       <formula>NOT(ISERROR(SEARCH("phone_number",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H101">
-    <cfRule type="containsText" dxfId="32" priority="6" operator="containsText" text="rooms">
+    <cfRule type="containsText" dxfId="30" priority="6" operator="containsText" text="rooms">
       <formula>NOT(ISERROR(SEARCH("rooms",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C101">
-    <cfRule type="expression" dxfId="31" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="7" stopIfTrue="1">
       <formula>ISBLANK(C1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D101">
-    <cfRule type="expression" dxfId="30" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="8" stopIfTrue="1">
       <formula>ISBLANK(D1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E101">
-    <cfRule type="expression" dxfId="29" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="9" stopIfTrue="1">
       <formula>ISBLANK(E1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F101">
-    <cfRule type="expression" dxfId="28" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="10" stopIfTrue="1">
       <formula>ISBLANK(F1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G101">
-    <cfRule type="expression" dxfId="27" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="11" stopIfTrue="1">
       <formula>ISBLANK(G1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H101">
-    <cfRule type="expression" dxfId="26" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="12" stopIfTrue="1">
       <formula>ISBLANK(H1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9027,19 +9028,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
     <col min="3" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9065,7 +9066,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>397</v>
       </c>
@@ -9091,7 +9092,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="270" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>399</v>
       </c>
@@ -9117,7 +9118,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>401</v>
       </c>
@@ -9143,7 +9144,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>403</v>
       </c>
@@ -9169,7 +9170,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>405</v>
       </c>
@@ -9195,7 +9196,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>406</v>
       </c>
@@ -9221,7 +9222,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>407</v>
       </c>
@@ -9247,7 +9248,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>409</v>
       </c>
@@ -9273,7 +9274,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>411</v>
       </c>
@@ -9299,7 +9300,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>413</v>
       </c>
@@ -9325,7 +9326,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>415</v>
       </c>
@@ -9351,7 +9352,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>417</v>
       </c>
@@ -9377,7 +9378,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>419</v>
       </c>
@@ -9405,62 +9406,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C101">
-    <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="start_date">
+    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="start_date">
       <formula>NOT(ISERROR(SEARCH("start_date",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D101">
-    <cfRule type="containsText" dxfId="24" priority="2" operator="containsText" text="end_date">
+    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="end_date">
       <formula>NOT(ISERROR(SEARCH("end_date",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E101">
-    <cfRule type="containsText" dxfId="23" priority="3" operator="containsText" text="price">
+    <cfRule type="containsText" dxfId="21" priority="3" operator="containsText" text="price">
       <formula>NOT(ISERROR(SEARCH("price",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F101">
-    <cfRule type="containsText" dxfId="22" priority="4" operator="containsText" text="location">
+    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="location">
       <formula>NOT(ISERROR(SEARCH("location",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G101">
-    <cfRule type="containsText" dxfId="21" priority="5" operator="containsText" text="phone_number">
+    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="phone_number">
       <formula>NOT(ISERROR(SEARCH("phone_number",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H101">
-    <cfRule type="containsText" dxfId="20" priority="6" operator="containsText" text="rooms">
+    <cfRule type="containsText" dxfId="18" priority="6" operator="containsText" text="rooms">
       <formula>NOT(ISERROR(SEARCH("rooms",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C101">
-    <cfRule type="expression" dxfId="19" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="7" stopIfTrue="1">
       <formula>ISBLANK(C1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D101">
-    <cfRule type="expression" dxfId="18" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="8" stopIfTrue="1">
       <formula>ISBLANK(D1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E101">
-    <cfRule type="expression" dxfId="17" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="9" stopIfTrue="1">
       <formula>ISBLANK(E1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F101">
-    <cfRule type="expression" dxfId="16" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="10" stopIfTrue="1">
       <formula>ISBLANK(F1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G101">
-    <cfRule type="expression" dxfId="15" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="11" stopIfTrue="1">
       <formula>ISBLANK(G1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H101">
-    <cfRule type="expression" dxfId="14" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
       <formula>ISBLANK(H1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9469,19 +9470,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
     <col min="3" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9509,62 +9510,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C101">
-    <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="start_date">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="start_date">
       <formula>NOT(ISERROR(SEARCH("start_date",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D101">
-    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="end_date">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="end_date">
       <formula>NOT(ISERROR(SEARCH("end_date",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E101">
-    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="price">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="price">
       <formula>NOT(ISERROR(SEARCH("price",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F101">
-    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="location">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="location">
       <formula>NOT(ISERROR(SEARCH("location",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G101">
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="phone_number">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="phone_number">
       <formula>NOT(ISERROR(SEARCH("phone_number",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H101">
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="rooms">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="rooms">
       <formula>NOT(ISERROR(SEARCH("rooms",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C101">
-    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
       <formula>ISBLANK(C1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D101">
-    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="8" stopIfTrue="1">
       <formula>ISBLANK(D1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E101">
-    <cfRule type="expression" dxfId="5" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="9" stopIfTrue="1">
       <formula>ISBLANK(E1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F101">
-    <cfRule type="expression" dxfId="4" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="10" stopIfTrue="1">
       <formula>ISBLANK(F1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G101">
-    <cfRule type="expression" dxfId="3" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="11" stopIfTrue="1">
       <formula>ISBLANK(G1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H101">
-    <cfRule type="expression" dxfId="2" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="12" stopIfTrue="1">
       <formula>ISBLANK(H1)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix some tagging examples
</commit_message>
<xml_diff>
--- a/data_utils/data_for_tagging.xlsx
+++ b/data_utils/data_for_tagging.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eliyasegev/PycharmProjects/traveliz/data_utils/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avishaya\PycharmProjects\traveliz\data_utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035CC488-B495-4AC1-BC97-4EE90BD6112B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="-57720" yWindow="-3795" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="facebook_posts_1" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1675" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="511">
   <si>
     <t>Post_id</t>
   </si>
@@ -2670,9 +2671,6 @@
     <t>3300 m</t>
   </si>
   <si>
-    <t>350, 490 d</t>
-  </si>
-  <si>
     <t>150 d</t>
   </si>
   <si>
@@ -2703,9 +2701,6 @@
     <t>1500 7d</t>
   </si>
   <si>
-    <t>300, 350 d</t>
-  </si>
-  <si>
     <t>500 3d</t>
   </si>
   <si>
@@ -2743,12 +2738,21 @@
   </si>
   <si>
     <t>200 d</t>
+  </si>
+  <si>
+    <t>350 p, 490 d</t>
+  </si>
+  <si>
+    <t>1500 d, 2200 d</t>
+  </si>
+  <si>
+    <t>300 2d, 350 d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2861,29 +2865,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="-5935432621049393351" xfId="2"/>
-    <cellStyle name="227581367215772297" xfId="1"/>
+    <cellStyle name="227581367215772297" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="-5935432621049393351" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="50">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3195,6 +3181,24 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3613,21 +3617,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
     <col min="3" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3653,7 +3657,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -3679,7 +3683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -3705,7 +3709,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -3731,7 +3735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -3757,7 +3761,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -3783,7 +3787,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -3809,7 +3813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -3835,7 +3839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="240" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -3861,7 +3865,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="288" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="270" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -3887,7 +3891,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="255" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
@@ -3913,7 +3917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
@@ -3939,7 +3943,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="255" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
@@ -3965,7 +3969,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>38</v>
       </c>
@@ -3979,7 +3983,7 @@
         <v>437</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>485</v>
+        <v>508</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>426</v>
@@ -3991,7 +3995,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -4017,7 +4021,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>42</v>
       </c>
@@ -4031,7 +4035,7 @@
         <v>441</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>439</v>
@@ -4043,7 +4047,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
@@ -4069,7 +4073,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>46</v>
       </c>
@@ -4083,7 +4087,7 @@
         <v>444</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>487</v>
+        <v>509</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>445</v>
@@ -4092,10 +4096,10 @@
         <v>543286986</v>
       </c>
       <c r="H18" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>48</v>
       </c>
@@ -4121,7 +4125,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>50</v>
       </c>
@@ -4147,7 +4151,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
@@ -4161,7 +4165,7 @@
         <v>11</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>426</v>
@@ -4173,7 +4177,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>54</v>
       </c>
@@ -4187,7 +4191,7 @@
         <v>437</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>448</v>
@@ -4195,11 +4199,11 @@
       <c r="G22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+      <c r="H22" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="180" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>56</v>
       </c>
@@ -4225,7 +4229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>58</v>
       </c>
@@ -4239,7 +4243,7 @@
         <v>11</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>426</v>
@@ -4251,7 +4255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>60</v>
       </c>
@@ -4265,7 +4269,7 @@
         <v>443</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>426</v>
@@ -4277,7 +4281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>62</v>
       </c>
@@ -4300,10 +4304,10 @@
         <v>14</v>
       </c>
       <c r="H26" s="4">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>64</v>
       </c>
@@ -4325,11 +4329,11 @@
       <c r="G27" s="4">
         <v>537295478</v>
       </c>
-      <c r="H27" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H27" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>66</v>
       </c>
@@ -4355,7 +4359,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>68</v>
       </c>
@@ -4381,7 +4385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>70</v>
       </c>
@@ -4407,7 +4411,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>72</v>
       </c>
@@ -4430,10 +4434,10 @@
         <v>14</v>
       </c>
       <c r="H31" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>74</v>
       </c>
@@ -4447,7 +4451,7 @@
         <v>11</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>13</v>
@@ -4459,7 +4463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>76</v>
       </c>
@@ -4485,7 +4489,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>78</v>
       </c>
@@ -4499,7 +4503,7 @@
         <v>461</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>462</v>
@@ -4511,7 +4515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="180" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>80</v>
       </c>
@@ -4525,7 +4529,7 @@
         <v>11</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>435</v>
@@ -4537,7 +4541,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>82</v>
       </c>
@@ -4551,7 +4555,7 @@
         <v>11</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>426</v>
@@ -4563,7 +4567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>84</v>
       </c>
@@ -4589,7 +4593,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>86</v>
       </c>
@@ -4615,7 +4619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>88</v>
       </c>
@@ -4638,10 +4642,10 @@
         <v>58448876</v>
       </c>
       <c r="H39" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>90</v>
       </c>
@@ -4655,7 +4659,7 @@
         <v>466</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>426</v>
@@ -4667,7 +4671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>92</v>
       </c>
@@ -4693,7 +4697,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>48</v>
       </c>
@@ -4719,7 +4723,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>94</v>
       </c>
@@ -4745,7 +4749,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>96</v>
       </c>
@@ -4759,7 +4763,7 @@
         <v>11</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>435</v>
@@ -4771,7 +4775,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>98</v>
       </c>
@@ -4785,7 +4789,7 @@
         <v>469</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>427</v>
@@ -4797,7 +4801,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>100</v>
       </c>
@@ -4823,7 +4827,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>102</v>
       </c>
@@ -4849,7 +4853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>104</v>
       </c>
@@ -4875,7 +4879,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>105</v>
       </c>
@@ -4889,7 +4893,7 @@
         <v>11</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>496</v>
+        <v>510</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>473</v>
@@ -4901,7 +4905,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>107</v>
       </c>
@@ -4915,7 +4919,7 @@
         <v>430</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>427</v>
@@ -4927,7 +4931,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>109</v>
       </c>
@@ -4953,7 +4957,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>111</v>
       </c>
@@ -4979,7 +4983,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>113</v>
       </c>
@@ -5005,7 +5009,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>115</v>
       </c>
@@ -5019,7 +5023,7 @@
         <v>425</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F54" s="4" t="s">
         <v>423</v>
@@ -5031,7 +5035,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="304" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" ht="285" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>117</v>
       </c>
@@ -5057,7 +5061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>119</v>
       </c>
@@ -5079,11 +5083,11 @@
       <c r="G56" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H56" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+      <c r="H56" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>121</v>
       </c>
@@ -5109,7 +5113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>123</v>
       </c>
@@ -5135,7 +5139,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>125</v>
       </c>
@@ -5152,16 +5156,16 @@
         <v>12</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="G59" s="4">
         <v>545510966</v>
       </c>
-      <c r="H59" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+      <c r="H59" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>127</v>
       </c>
@@ -5178,7 +5182,7 @@
         <v>12</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="G60" s="4">
         <v>503200148</v>
@@ -5187,7 +5191,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>129</v>
       </c>
@@ -5201,7 +5205,7 @@
         <v>11</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F61" s="4" t="s">
         <v>426</v>
@@ -5213,7 +5217,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="240" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" ht="225" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>131</v>
       </c>
@@ -5227,7 +5231,7 @@
         <v>11</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="F62" s="4" t="s">
         <v>426</v>
@@ -5239,7 +5243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>133</v>
       </c>
@@ -5250,10 +5254,10 @@
         <v>452</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="F63" s="4" t="s">
         <v>431</v>
@@ -5262,10 +5266,10 @@
         <v>502290056</v>
       </c>
       <c r="H63" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>135</v>
       </c>
@@ -5273,7 +5277,7 @@
         <v>136</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>464</v>
@@ -5291,7 +5295,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>137</v>
       </c>
@@ -5302,7 +5306,7 @@
         <v>429</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>12</v>
@@ -5317,7 +5321,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="304" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" ht="285" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>139</v>
       </c>
@@ -5325,13 +5329,13 @@
         <v>140</v>
       </c>
       <c r="C66" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="E66" s="4" t="s">
         <v>507</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>508</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>509</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>431</v>
@@ -5343,7 +5347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>141</v>
       </c>
@@ -5357,7 +5361,7 @@
         <v>11</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F67" s="4" t="s">
         <v>426</v>
@@ -5369,7 +5373,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>142</v>
       </c>
@@ -5395,7 +5399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>144</v>
       </c>
@@ -5418,10 +5422,10 @@
         <v>14</v>
       </c>
       <c r="H69" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>146</v>
       </c>
@@ -5447,7 +5451,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>148</v>
       </c>
@@ -5473,7 +5477,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>150</v>
       </c>
@@ -5499,7 +5503,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>152</v>
       </c>
@@ -5525,7 +5529,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>154</v>
       </c>
@@ -5551,7 +5555,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>156</v>
       </c>
@@ -5577,7 +5581,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>158</v>
       </c>
@@ -5603,7 +5607,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>160</v>
       </c>
@@ -5629,7 +5633,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="304" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" ht="315" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>162</v>
       </c>
@@ -5655,7 +5659,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>164</v>
       </c>
@@ -5681,7 +5685,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>166</v>
       </c>
@@ -5707,7 +5711,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>168</v>
       </c>
@@ -5733,7 +5737,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>170</v>
       </c>
@@ -5759,7 +5763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>172</v>
       </c>
@@ -5785,7 +5789,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>174</v>
       </c>
@@ -5811,7 +5815,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>176</v>
       </c>
@@ -5837,7 +5841,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>178</v>
       </c>
@@ -5863,7 +5867,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>180</v>
       </c>
@@ -5889,7 +5893,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>182</v>
       </c>
@@ -5915,7 +5919,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>184</v>
       </c>
@@ -5941,7 +5945,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>186</v>
       </c>
@@ -5967,7 +5971,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>188</v>
       </c>
@@ -5993,7 +5997,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>190</v>
       </c>
@@ -6019,7 +6023,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>192</v>
       </c>
@@ -6045,7 +6049,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>194</v>
       </c>
@@ -6071,7 +6075,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>196</v>
       </c>
@@ -6097,7 +6101,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>198</v>
       </c>
@@ -6123,7 +6127,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>200</v>
       </c>
@@ -6149,7 +6153,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>202</v>
       </c>
@@ -6175,7 +6179,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="400" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" ht="375" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>204</v>
       </c>
@@ -6201,7 +6205,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>206</v>
       </c>
@@ -6227,7 +6231,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>208</v>
       </c>
@@ -6315,12 +6319,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="start_date">
+    <cfRule type="containsText" dxfId="37" priority="1" operator="containsText" text="start_date">
       <formula>NOT(ISERROR(SEARCH("start_date",D45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="2" stopIfTrue="1">
       <formula>ISBLANK(D45)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6329,19 +6333,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
     <col min="3" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6367,7 +6371,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>210</v>
       </c>
@@ -6393,7 +6397,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>212</v>
       </c>
@@ -6419,7 +6423,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>214</v>
       </c>
@@ -6445,7 +6449,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>216</v>
       </c>
@@ -6471,7 +6475,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="288" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="285" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>218</v>
       </c>
@@ -6497,7 +6501,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>220</v>
       </c>
@@ -6523,7 +6527,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>222</v>
       </c>
@@ -6549,7 +6553,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>224</v>
       </c>
@@ -6575,7 +6579,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="285" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>226</v>
       </c>
@@ -6601,7 +6605,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="270" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>228</v>
       </c>
@@ -6627,7 +6631,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="255" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>230</v>
       </c>
@@ -6653,7 +6657,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>232</v>
       </c>
@@ -6679,7 +6683,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>234</v>
       </c>
@@ -6705,7 +6709,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>236</v>
       </c>
@@ -6731,7 +6735,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>237</v>
       </c>
@@ -6757,7 +6761,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>239</v>
       </c>
@@ -6783,7 +6787,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>240</v>
       </c>
@@ -6809,7 +6813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>242</v>
       </c>
@@ -6835,7 +6839,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>244</v>
       </c>
@@ -6861,7 +6865,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>245</v>
       </c>
@@ -6887,7 +6891,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>247</v>
       </c>
@@ -6913,7 +6917,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="288" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="270" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>249</v>
       </c>
@@ -6939,7 +6943,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>251</v>
       </c>
@@ -6965,7 +6969,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>253</v>
       </c>
@@ -6991,7 +6995,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>255</v>
       </c>
@@ -7017,7 +7021,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="255" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>257</v>
       </c>
@@ -7043,7 +7047,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>259</v>
       </c>
@@ -7069,7 +7073,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>261</v>
       </c>
@@ -7095,7 +7099,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>263</v>
       </c>
@@ -7121,7 +7125,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>264</v>
       </c>
@@ -7147,7 +7151,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>266</v>
       </c>
@@ -7173,7 +7177,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>268</v>
       </c>
@@ -7199,7 +7203,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>269</v>
       </c>
@@ -7225,7 +7229,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>271</v>
       </c>
@@ -7251,7 +7255,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>273</v>
       </c>
@@ -7277,7 +7281,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>274</v>
       </c>
@@ -7303,7 +7307,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>276</v>
       </c>
@@ -7329,7 +7333,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>278</v>
       </c>
@@ -7355,7 +7359,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" ht="180" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>280</v>
       </c>
@@ -7381,7 +7385,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>282</v>
       </c>
@@ -7407,7 +7411,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>284</v>
       </c>
@@ -7433,7 +7437,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>286</v>
       </c>
@@ -7459,7 +7463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>288</v>
       </c>
@@ -7485,7 +7489,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>290</v>
       </c>
@@ -7511,7 +7515,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>292</v>
       </c>
@@ -7537,7 +7541,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>294</v>
       </c>
@@ -7563,7 +7567,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="304" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" ht="285" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>296</v>
       </c>
@@ -7589,7 +7593,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" ht="255" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>298</v>
       </c>
@@ -7615,7 +7619,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>300</v>
       </c>
@@ -7641,7 +7645,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>301</v>
       </c>
@@ -7667,7 +7671,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="240" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>303</v>
       </c>
@@ -7693,7 +7697,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>305</v>
       </c>
@@ -7719,7 +7723,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>307</v>
       </c>
@@ -7745,7 +7749,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>309</v>
       </c>
@@ -7771,7 +7775,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>311</v>
       </c>
@@ -7797,7 +7801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>313</v>
       </c>
@@ -7823,7 +7827,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>315</v>
       </c>
@@ -7849,7 +7853,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="320" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" ht="330" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>317</v>
       </c>
@@ -7875,7 +7879,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>319</v>
       </c>
@@ -7901,7 +7905,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>321</v>
       </c>
@@ -7925,7 +7929,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>322</v>
       </c>
@@ -7951,7 +7955,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>324</v>
       </c>
@@ -7977,7 +7981,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>326</v>
       </c>
@@ -8001,7 +8005,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" ht="285" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>327</v>
       </c>
@@ -8027,7 +8031,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>329</v>
       </c>
@@ -8053,7 +8057,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" ht="180" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>331</v>
       </c>
@@ -8079,7 +8083,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>333</v>
       </c>
@@ -8105,7 +8109,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>335</v>
       </c>
@@ -8131,7 +8135,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>337</v>
       </c>
@@ -8157,7 +8161,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>338</v>
       </c>
@@ -8183,7 +8187,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>340</v>
       </c>
@@ -8209,7 +8213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" ht="390" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>342</v>
       </c>
@@ -8235,7 +8239,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>344</v>
       </c>
@@ -8261,7 +8265,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>346</v>
       </c>
@@ -8287,7 +8291,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" ht="180" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>348</v>
       </c>
@@ -8313,7 +8317,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>350</v>
       </c>
@@ -8337,7 +8341,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" ht="180" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>351</v>
       </c>
@@ -8363,7 +8367,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>353</v>
       </c>
@@ -8389,7 +8393,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>355</v>
       </c>
@@ -8415,7 +8419,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>357</v>
       </c>
@@ -8441,7 +8445,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>359</v>
       </c>
@@ -8467,7 +8471,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>360</v>
       </c>
@@ -8493,7 +8497,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>362</v>
       </c>
@@ -8519,7 +8523,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>364</v>
       </c>
@@ -8545,7 +8549,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>366</v>
       </c>
@@ -8571,7 +8575,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>368</v>
       </c>
@@ -8597,7 +8601,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>370</v>
       </c>
@@ -8623,7 +8627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>372</v>
       </c>
@@ -8649,7 +8653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>374</v>
       </c>
@@ -8675,7 +8679,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>375</v>
       </c>
@@ -8701,7 +8705,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="352" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" ht="345" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>377</v>
       </c>
@@ -8727,7 +8731,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>379</v>
       </c>
@@ -8753,7 +8757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>381</v>
       </c>
@@ -8779,7 +8783,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>383</v>
       </c>
@@ -8805,7 +8809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>385</v>
       </c>
@@ -8831,7 +8835,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>387</v>
       </c>
@@ -8857,7 +8861,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>389</v>
       </c>
@@ -8883,7 +8887,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>391</v>
       </c>
@@ -8909,7 +8913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>393</v>
       </c>
@@ -8935,7 +8939,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>395</v>
       </c>
@@ -8963,62 +8967,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C101">
-    <cfRule type="containsText" dxfId="37" priority="1" operator="containsText" text="start_date">
+    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="start_date">
       <formula>NOT(ISERROR(SEARCH("start_date",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D101">
-    <cfRule type="containsText" dxfId="36" priority="2" operator="containsText" text="end_date">
+    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="end_date">
       <formula>NOT(ISERROR(SEARCH("end_date",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E101">
-    <cfRule type="containsText" dxfId="35" priority="3" operator="containsText" text="price">
+    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="price">
       <formula>NOT(ISERROR(SEARCH("price",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F101">
-    <cfRule type="containsText" dxfId="34" priority="4" operator="containsText" text="location">
+    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="location">
       <formula>NOT(ISERROR(SEARCH("location",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G101">
-    <cfRule type="containsText" dxfId="33" priority="5" operator="containsText" text="phone_number">
+    <cfRule type="containsText" dxfId="31" priority="5" operator="containsText" text="phone_number">
       <formula>NOT(ISERROR(SEARCH("phone_number",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H101">
-    <cfRule type="containsText" dxfId="32" priority="6" operator="containsText" text="rooms">
+    <cfRule type="containsText" dxfId="30" priority="6" operator="containsText" text="rooms">
       <formula>NOT(ISERROR(SEARCH("rooms",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C101">
-    <cfRule type="expression" dxfId="31" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="7" stopIfTrue="1">
       <formula>ISBLANK(C1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D101">
-    <cfRule type="expression" dxfId="30" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="8" stopIfTrue="1">
       <formula>ISBLANK(D1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E101">
-    <cfRule type="expression" dxfId="29" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="9" stopIfTrue="1">
       <formula>ISBLANK(E1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F101">
-    <cfRule type="expression" dxfId="28" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="10" stopIfTrue="1">
       <formula>ISBLANK(F1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G101">
-    <cfRule type="expression" dxfId="27" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="11" stopIfTrue="1">
       <formula>ISBLANK(G1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H101">
-    <cfRule type="expression" dxfId="26" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="12" stopIfTrue="1">
       <formula>ISBLANK(H1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9027,19 +9031,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
     <col min="3" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9065,7 +9069,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>397</v>
       </c>
@@ -9091,7 +9095,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="270" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>399</v>
       </c>
@@ -9117,7 +9121,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>401</v>
       </c>
@@ -9143,7 +9147,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>403</v>
       </c>
@@ -9169,7 +9173,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>405</v>
       </c>
@@ -9195,7 +9199,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>406</v>
       </c>
@@ -9221,7 +9225,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>407</v>
       </c>
@@ -9247,7 +9251,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>409</v>
       </c>
@@ -9273,7 +9277,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>411</v>
       </c>
@@ -9299,7 +9303,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>413</v>
       </c>
@@ -9325,7 +9329,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>415</v>
       </c>
@@ -9351,7 +9355,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>417</v>
       </c>
@@ -9377,7 +9381,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>419</v>
       </c>
@@ -9405,62 +9409,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C101">
-    <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="start_date">
+    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="start_date">
       <formula>NOT(ISERROR(SEARCH("start_date",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D101">
-    <cfRule type="containsText" dxfId="24" priority="2" operator="containsText" text="end_date">
+    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="end_date">
       <formula>NOT(ISERROR(SEARCH("end_date",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E101">
-    <cfRule type="containsText" dxfId="23" priority="3" operator="containsText" text="price">
+    <cfRule type="containsText" dxfId="21" priority="3" operator="containsText" text="price">
       <formula>NOT(ISERROR(SEARCH("price",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F101">
-    <cfRule type="containsText" dxfId="22" priority="4" operator="containsText" text="location">
+    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="location">
       <formula>NOT(ISERROR(SEARCH("location",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G101">
-    <cfRule type="containsText" dxfId="21" priority="5" operator="containsText" text="phone_number">
+    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="phone_number">
       <formula>NOT(ISERROR(SEARCH("phone_number",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H101">
-    <cfRule type="containsText" dxfId="20" priority="6" operator="containsText" text="rooms">
+    <cfRule type="containsText" dxfId="18" priority="6" operator="containsText" text="rooms">
       <formula>NOT(ISERROR(SEARCH("rooms",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C101">
-    <cfRule type="expression" dxfId="19" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="7" stopIfTrue="1">
       <formula>ISBLANK(C1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D101">
-    <cfRule type="expression" dxfId="18" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="8" stopIfTrue="1">
       <formula>ISBLANK(D1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E101">
-    <cfRule type="expression" dxfId="17" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="9" stopIfTrue="1">
       <formula>ISBLANK(E1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F101">
-    <cfRule type="expression" dxfId="16" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="10" stopIfTrue="1">
       <formula>ISBLANK(F1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G101">
-    <cfRule type="expression" dxfId="15" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="11" stopIfTrue="1">
       <formula>ISBLANK(G1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H101">
-    <cfRule type="expression" dxfId="14" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
       <formula>ISBLANK(H1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9469,19 +9473,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
     <col min="3" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9509,62 +9513,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C101">
-    <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="start_date">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="start_date">
       <formula>NOT(ISERROR(SEARCH("start_date",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D101">
-    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="end_date">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="end_date">
       <formula>NOT(ISERROR(SEARCH("end_date",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E101">
-    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="price">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="price">
       <formula>NOT(ISERROR(SEARCH("price",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F101">
-    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="location">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="location">
       <formula>NOT(ISERROR(SEARCH("location",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G101">
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="phone_number">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="phone_number">
       <formula>NOT(ISERROR(SEARCH("phone_number",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H101">
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="rooms">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="rooms">
       <formula>NOT(ISERROR(SEARCH("rooms",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C101">
-    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
       <formula>ISBLANK(C1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D101">
-    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="8" stopIfTrue="1">
       <formula>ISBLANK(D1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E101">
-    <cfRule type="expression" dxfId="5" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="9" stopIfTrue="1">
       <formula>ISBLANK(E1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F101">
-    <cfRule type="expression" dxfId="4" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="10" stopIfTrue="1">
       <formula>ISBLANK(F1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G101">
-    <cfRule type="expression" dxfId="3" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="11" stopIfTrue="1">
       <formula>ISBLANK(G1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H101">
-    <cfRule type="expression" dxfId="2" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="12" stopIfTrue="1">
       <formula>ISBLANK(H1)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update tagging excel and teset db
</commit_message>
<xml_diff>
--- a/data_utils/data_for_tagging.xlsx
+++ b/data_utils/data_for_tagging.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avishaya\PycharmProjects\traveliz\data_utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Y\PycharmProjects\traveliz\data_utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035CC488-B495-4AC1-BC97-4EE90BD6112B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217CB18D-672E-40EE-AD3E-0C4688B83B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-3795" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="facebook_posts_1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="510">
   <si>
     <t>Post_id</t>
   </si>
@@ -2590,9 +2590,6 @@
     <t>30.11.2021</t>
   </si>
   <si>
-    <t>05.12.201</t>
-  </si>
-  <si>
     <t>שדה אילן</t>
   </si>
   <si>
@@ -2674,9 +2671,6 @@
     <t>150 d</t>
   </si>
   <si>
-    <t>1500, 2200 d</t>
-  </si>
-  <si>
     <t>8750 m</t>
   </si>
   <si>
@@ -2747,6 +2741,9 @@
   </si>
   <si>
     <t>300 2d, 350 d</t>
+  </si>
+  <si>
+    <t>05.12.2021</t>
   </si>
 </sst>
 </file>
@@ -3620,8 +3617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3671,7 +3668,7 @@
         <v>422</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>423</v>
@@ -3775,7 +3772,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>427</v>
@@ -3801,7 +3798,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>427</v>
@@ -3827,7 +3824,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>428</v>
@@ -3853,7 +3850,7 @@
         <v>430</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>13</v>
@@ -3905,7 +3902,7 @@
         <v>11</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>426</v>
@@ -3957,7 +3954,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>435</v>
@@ -3983,7 +3980,7 @@
         <v>437</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>426</v>
@@ -4035,7 +4032,7 @@
         <v>441</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>439</v>
@@ -4087,7 +4084,7 @@
         <v>444</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>445</v>
@@ -4165,7 +4162,7 @@
         <v>11</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>426</v>
@@ -4191,7 +4188,7 @@
         <v>437</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>486</v>
+        <v>507</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>448</v>
@@ -4243,7 +4240,7 @@
         <v>11</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>426</v>
@@ -4269,7 +4266,7 @@
         <v>443</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>426</v>
@@ -4451,7 +4448,7 @@
         <v>11</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>13</v>
@@ -4474,13 +4471,13 @@
         <v>457</v>
       </c>
       <c r="D33" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>458</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>459</v>
       </c>
       <c r="G33" s="4">
         <v>528316179</v>
@@ -4497,16 +4494,16 @@
         <v>79</v>
       </c>
       <c r="C34" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>460</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="E34" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>461</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>491</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>462</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>14</v>
@@ -4529,7 +4526,7 @@
         <v>11</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>435</v>
@@ -4555,7 +4552,7 @@
         <v>11</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>426</v>
@@ -4601,10 +4598,10 @@
         <v>87</v>
       </c>
       <c r="C38" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>463</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>464</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>12</v>
@@ -4636,7 +4633,7 @@
         <v>12</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G39" s="4">
         <v>58448876</v>
@@ -4656,10 +4653,10 @@
         <v>455</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>426</v>
@@ -4740,7 +4737,7 @@
         <v>12</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>14</v>
@@ -4763,13 +4760,13 @@
         <v>11</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>435</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>15</v>
@@ -4783,13 +4780,13 @@
         <v>99</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>427</v>
@@ -4809,7 +4806,7 @@
         <v>101</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>457</v>
@@ -4844,7 +4841,7 @@
         <v>12</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>14</v>
@@ -4893,10 +4890,10 @@
         <v>11</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>14</v>
@@ -4919,7 +4916,7 @@
         <v>430</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>427</v>
@@ -4939,10 +4936,10 @@
         <v>110</v>
       </c>
       <c r="C51" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>474</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>475</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>12</v>
@@ -5017,13 +5014,13 @@
         <v>116</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>425</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F54" s="4" t="s">
         <v>423</v>
@@ -5049,7 +5046,7 @@
         <v>11</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F55" s="4" t="s">
         <v>423</v>
@@ -5121,7 +5118,7 @@
         <v>124</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>422</v>
@@ -5156,7 +5153,7 @@
         <v>12</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G59" s="4">
         <v>545510966</v>
@@ -5182,7 +5179,7 @@
         <v>12</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G60" s="4">
         <v>503200148</v>
@@ -5205,7 +5202,7 @@
         <v>11</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="F61" s="4" t="s">
         <v>426</v>
@@ -5231,7 +5228,7 @@
         <v>11</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="F62" s="4" t="s">
         <v>426</v>
@@ -5254,10 +5251,10 @@
         <v>452</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F63" s="4" t="s">
         <v>431</v>
@@ -5277,10 +5274,10 @@
         <v>136</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>12</v>
@@ -5306,7 +5303,7 @@
         <v>429</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>12</v>
@@ -5329,13 +5326,13 @@
         <v>140</v>
       </c>
       <c r="C66" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="E66" s="4" t="s">
         <v>505</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>506</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>507</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>431</v>
@@ -5361,7 +5358,7 @@
         <v>11</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="F67" s="4" t="s">
         <v>426</v>
@@ -5381,7 +5378,7 @@
         <v>143</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>444</v>

</xml_diff>

<commit_message>
small adaptations for refactor rooms
</commit_message>
<xml_diff>
--- a/data_utils/data_for_tagging.xlsx
+++ b/data_utils/data_for_tagging.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eliyasegev/PycharmProjects/traveliz/data_utils/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avishaya\PycharmProjects\traveliz\data_utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5338BFB4-0F7D-4BFD-8394-621A3FC59F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="500" windowWidth="28500" windowHeight="16280"/>
+    <workbookView xWindow="-57720" yWindow="-3795" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="facebook" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1647" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="516">
   <si>
     <t>Post_id</t>
   </si>
@@ -2796,11 +2796,17 @@
 המון טבע מסביב.....
 https://www.facebook.com/476757013074004/posts/1040673753348991/</t>
   </si>
+  <si>
+    <t>None s</t>
+  </si>
+  <si>
+    <t>4 s</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2939,12 +2945,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="-3451930801534778880" xfId="1"/>
-    <cellStyle name="-5935432621049393351" xfId="6"/>
-    <cellStyle name="-6133241657024543279" xfId="4"/>
-    <cellStyle name="-729664007974769509" xfId="2"/>
-    <cellStyle name="-918871240910345814" xfId="3"/>
-    <cellStyle name="227581367215772297" xfId="5"/>
+    <cellStyle name="227581367215772297" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="-3451930801534778880" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="-5935432621049393351" xfId="6" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="-6133241657024543279" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="-729664007974769509" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="-918871240910345814" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="50">
@@ -3400,77 +3406,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3760,21 +3701,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H214"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
     <col min="3" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3800,7 +3741,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -3822,11 +3763,11 @@
       <c r="G2" s="6">
         <v>544747880</v>
       </c>
-      <c r="H2" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H2" s="6" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
@@ -3852,7 +3793,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
@@ -3878,7 +3819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
@@ -3904,7 +3845,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
@@ -3930,7 +3871,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -3956,7 +3897,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
@@ -3982,7 +3923,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="240" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -4008,7 +3949,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="288" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="270" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
@@ -4034,7 +3975,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="255" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
@@ -4060,7 +4001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
@@ -4086,7 +4027,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="255" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>26</v>
       </c>
@@ -4112,7 +4053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
@@ -4138,7 +4079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>29</v>
       </c>
@@ -4164,7 +4105,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>30</v>
       </c>
@@ -4190,7 +4131,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>31</v>
       </c>
@@ -4216,7 +4157,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>33</v>
       </c>
@@ -4242,7 +4183,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>34</v>
       </c>
@@ -4268,7 +4209,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>35</v>
       </c>
@@ -4294,7 +4235,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>36</v>
       </c>
@@ -4320,7 +4261,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>37</v>
       </c>
@@ -4346,7 +4287,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="180" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>38</v>
       </c>
@@ -4372,7 +4313,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>39</v>
       </c>
@@ -4398,7 +4339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>40</v>
       </c>
@@ -4420,11 +4361,11 @@
       <c r="G25" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+      <c r="H25" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>42</v>
       </c>
@@ -4450,7 +4391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>43</v>
       </c>
@@ -4476,7 +4417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>45</v>
       </c>
@@ -4502,7 +4443,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>47</v>
       </c>
@@ -4528,7 +4469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>48</v>
       </c>
@@ -4554,7 +4495,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="403" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="403.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>49</v>
       </c>
@@ -4580,7 +4521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>50</v>
       </c>
@@ -4606,7 +4547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>51</v>
       </c>
@@ -4632,7 +4573,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>52</v>
       </c>
@@ -4658,7 +4599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>53</v>
       </c>
@@ -4684,7 +4625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>54</v>
       </c>
@@ -4710,7 +4651,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>55</v>
       </c>
@@ -4736,7 +4677,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>56</v>
       </c>
@@ -4762,7 +4703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>57</v>
       </c>
@@ -4788,7 +4729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>58</v>
       </c>
@@ -4814,7 +4755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>59</v>
       </c>
@@ -4840,7 +4781,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>34</v>
       </c>
@@ -4866,7 +4807,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>61</v>
       </c>
@@ -4892,7 +4833,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>63</v>
       </c>
@@ -4918,7 +4859,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>64</v>
       </c>
@@ -4944,7 +4885,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>65</v>
       </c>
@@ -4970,7 +4911,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>66</v>
       </c>
@@ -4996,7 +4937,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>67</v>
       </c>
@@ -5022,7 +4963,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>68</v>
       </c>
@@ -5048,7 +4989,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>69</v>
       </c>
@@ -5074,7 +5015,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>70</v>
       </c>
@@ -5100,7 +5041,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>71</v>
       </c>
@@ -5126,7 +5067,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>73</v>
       </c>
@@ -5152,7 +5093,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>75</v>
       </c>
@@ -5178,7 +5119,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>77</v>
       </c>
@@ -5204,7 +5145,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>78</v>
       </c>
@@ -5230,7 +5171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>79</v>
       </c>
@@ -5256,7 +5197,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>80</v>
       </c>
@@ -5282,7 +5223,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>81</v>
       </c>
@@ -5308,7 +5249,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>82</v>
       </c>
@@ -5334,7 +5275,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" ht="160.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>83</v>
       </c>
@@ -5360,7 +5301,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="240" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" ht="225" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>84</v>
       </c>
@@ -5386,7 +5327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>85</v>
       </c>
@@ -5412,7 +5353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>86</v>
       </c>
@@ -5438,7 +5379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="172" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" ht="172.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>87</v>
       </c>
@@ -5464,7 +5405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="304" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" ht="285" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>88</v>
       </c>
@@ -5490,7 +5431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="210" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" ht="210" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>89</v>
       </c>
@@ -5516,7 +5457,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>90</v>
       </c>
@@ -5542,7 +5483,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>91</v>
       </c>
@@ -5568,7 +5509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>92</v>
       </c>
@@ -5594,7 +5535,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>94</v>
       </c>
@@ -5620,7 +5561,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="400" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>96</v>
       </c>
@@ -5646,7 +5587,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>98</v>
       </c>
@@ -5672,7 +5613,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>100</v>
       </c>
@@ -5698,7 +5639,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="320" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>102</v>
       </c>
@@ -5724,7 +5665,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>104</v>
       </c>
@@ -5750,7 +5691,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="304" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>106</v>
       </c>
@@ -5776,7 +5717,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" ht="409.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>108</v>
       </c>
@@ -5802,7 +5743,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>110</v>
       </c>
@@ -5828,7 +5769,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>112</v>
       </c>
@@ -5854,7 +5795,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>114</v>
       </c>
@@ -5880,7 +5821,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>116</v>
       </c>
@@ -5906,7 +5847,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>118</v>
       </c>
@@ -5932,7 +5873,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>120</v>
       </c>
@@ -5958,7 +5899,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>122</v>
       </c>
@@ -5984,7 +5925,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>124</v>
       </c>
@@ -6010,7 +5951,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>126</v>
       </c>
@@ -6036,7 +5977,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>128</v>
       </c>
@@ -6062,7 +6003,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>130</v>
       </c>
@@ -6088,7 +6029,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>132</v>
       </c>
@@ -6114,7 +6055,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="240" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>134</v>
       </c>
@@ -6140,7 +6081,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>136</v>
       </c>
@@ -6166,7 +6107,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>138</v>
       </c>
@@ -6192,7 +6133,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>140</v>
       </c>
@@ -6218,7 +6159,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>142</v>
       </c>
@@ -6244,7 +6185,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="288" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>144</v>
       </c>
@@ -6270,7 +6211,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="384" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>146</v>
       </c>
@@ -6296,7 +6237,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>148</v>
       </c>
@@ -6322,7 +6263,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" ht="375" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>150</v>
       </c>
@@ -6348,7 +6289,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>152</v>
       </c>
@@ -6374,7 +6315,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>154</v>
       </c>
@@ -6400,7 +6341,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>156</v>
       </c>
@@ -6426,7 +6367,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>158</v>
       </c>
@@ -6452,7 +6393,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="240" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>160</v>
       </c>
@@ -6478,7 +6419,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>162</v>
       </c>
@@ -6504,7 +6445,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" ht="285" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>164</v>
       </c>
@@ -6530,7 +6471,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>166</v>
       </c>
@@ -6556,7 +6497,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="240" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>168</v>
       </c>
@@ -6582,7 +6523,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>170</v>
       </c>
@@ -6608,7 +6549,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="336" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" ht="285" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>172</v>
       </c>
@@ -6634,7 +6575,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" ht="270" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>174</v>
       </c>
@@ -6660,7 +6601,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" ht="255" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>176</v>
       </c>
@@ -6686,7 +6627,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>178</v>
       </c>
@@ -6712,7 +6653,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>180</v>
       </c>
@@ -6738,7 +6679,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>182</v>
       </c>
@@ -6764,7 +6705,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>183</v>
       </c>
@@ -6790,7 +6731,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="288" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>185</v>
       </c>
@@ -6816,7 +6757,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>186</v>
       </c>
@@ -6842,7 +6783,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>188</v>
       </c>
@@ -6868,7 +6809,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>190</v>
       </c>
@@ -6894,7 +6835,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>191</v>
       </c>
@@ -6920,7 +6861,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>193</v>
       </c>
@@ -6946,7 +6887,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" ht="270" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>195</v>
       </c>
@@ -6972,7 +6913,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>197</v>
       </c>
@@ -6998,7 +6939,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="336" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>199</v>
       </c>
@@ -7024,7 +6965,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>201</v>
       </c>
@@ -7050,7 +6991,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" ht="255" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>203</v>
       </c>
@@ -7076,7 +7017,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>205</v>
       </c>
@@ -7102,7 +7043,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>207</v>
       </c>
@@ -7128,7 +7069,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>209</v>
       </c>
@@ -7154,7 +7095,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>210</v>
       </c>
@@ -7180,7 +7121,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>212</v>
       </c>
@@ -7206,7 +7147,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>214</v>
       </c>
@@ -7232,7 +7173,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>215</v>
       </c>
@@ -7258,7 +7199,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>217</v>
       </c>
@@ -7284,7 +7225,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>219</v>
       </c>
@@ -7310,7 +7251,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="336" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>220</v>
       </c>
@@ -7336,7 +7277,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>222</v>
       </c>
@@ -7362,7 +7303,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>224</v>
       </c>
@@ -7388,7 +7329,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" ht="180" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>226</v>
       </c>
@@ -7414,7 +7355,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>228</v>
       </c>
@@ -7440,7 +7381,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>230</v>
       </c>
@@ -7466,7 +7407,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>232</v>
       </c>
@@ -7492,7 +7433,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>234</v>
       </c>
@@ -7518,7 +7459,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>236</v>
       </c>
@@ -7544,7 +7485,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>238</v>
       </c>
@@ -7570,7 +7511,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>240</v>
       </c>
@@ -7596,7 +7537,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8" ht="285" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>242</v>
       </c>
@@ -7622,7 +7563,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="149" spans="1:8" ht="352" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8" ht="255" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>244</v>
       </c>
@@ -7648,7 +7589,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="150" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>246</v>
       </c>
@@ -7674,7 +7615,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="151" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>247</v>
       </c>
@@ -7700,7 +7641,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>249</v>
       </c>
@@ -7726,7 +7667,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="153" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>251</v>
       </c>
@@ -7752,7 +7693,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="154" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>253</v>
       </c>
@@ -7778,7 +7719,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="155" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8" ht="120" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>255</v>
       </c>
@@ -7804,7 +7745,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="156" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>257</v>
       </c>
@@ -7830,7 +7771,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="157" spans="1:8" ht="400" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>259</v>
       </c>
@@ -7856,7 +7797,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="158" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>261</v>
       </c>
@@ -7882,7 +7823,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="159" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:8" ht="330" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>263</v>
       </c>
@@ -7908,7 +7849,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="160" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>265</v>
       </c>
@@ -7934,7 +7875,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="161" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>267</v>
       </c>
@@ -7958,7 +7899,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="162" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>268</v>
       </c>
@@ -7984,7 +7925,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="163" spans="1:8" ht="320" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>270</v>
       </c>
@@ -8010,7 +7951,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="164" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>272</v>
       </c>
@@ -8034,7 +7975,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="165" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" ht="285" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>273</v>
       </c>
@@ -8060,7 +8001,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="166" spans="1:8" ht="240" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>275</v>
       </c>
@@ -8086,7 +8027,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="167" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" ht="180" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>277</v>
       </c>
@@ -8112,7 +8053,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>279</v>
       </c>
@@ -8138,7 +8079,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="169" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>281</v>
       </c>
@@ -8164,7 +8105,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="170" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>283</v>
       </c>
@@ -8190,7 +8131,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>284</v>
       </c>
@@ -8216,7 +8157,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="172" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>286</v>
       </c>
@@ -8242,7 +8183,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="173" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" ht="390" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>288</v>
       </c>
@@ -8268,7 +8209,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="174" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>290</v>
       </c>
@@ -8294,7 +8235,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="175" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>292</v>
       </c>
@@ -8320,7 +8261,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="176" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" ht="180" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>294</v>
       </c>
@@ -8346,7 +8287,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="177" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>296</v>
       </c>
@@ -8370,7 +8311,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="178" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8" ht="180" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>297</v>
       </c>
@@ -8396,7 +8337,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="179" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>299</v>
       </c>
@@ -8422,7 +8363,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="180" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>301</v>
       </c>
@@ -8448,7 +8389,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="181" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>303</v>
       </c>
@@ -8474,7 +8415,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>305</v>
       </c>
@@ -8500,7 +8441,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>306</v>
       </c>
@@ -8526,7 +8467,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>308</v>
       </c>
@@ -8552,7 +8493,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>310</v>
       </c>
@@ -8578,7 +8519,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>312</v>
       </c>
@@ -8604,7 +8545,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="187" spans="1:8" ht="384" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>314</v>
       </c>
@@ -8630,7 +8571,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="188" spans="1:8" ht="384" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>316</v>
       </c>
@@ -8656,7 +8597,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="189" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>318</v>
       </c>
@@ -8682,7 +8623,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="190" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>320</v>
       </c>
@@ -8708,7 +8649,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="191" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>321</v>
       </c>
@@ -8734,7 +8675,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="192" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:8" ht="345" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>323</v>
       </c>
@@ -8760,7 +8701,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="193" spans="1:8" ht="256" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>325</v>
       </c>
@@ -8786,7 +8727,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="194" spans="1:8" ht="400" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:8" ht="135" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>327</v>
       </c>
@@ -8812,7 +8753,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="195" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>329</v>
       </c>
@@ -8838,7 +8779,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="196" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>331</v>
       </c>
@@ -8864,7 +8805,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="197" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>333</v>
       </c>
@@ -8890,7 +8831,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="198" spans="1:8" ht="240" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>335</v>
       </c>
@@ -8916,7 +8857,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="199" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>337</v>
       </c>
@@ -8942,7 +8883,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="200" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>339</v>
       </c>
@@ -8968,7 +8909,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="201" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
         <v>341</v>
       </c>
@@ -8994,7 +8935,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="202" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:8" ht="105" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>343</v>
       </c>
@@ -9020,7 +8961,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="203" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:8" ht="270" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
         <v>345</v>
       </c>
@@ -9046,7 +8987,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="204" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>347</v>
       </c>
@@ -9072,7 +9013,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="205" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:8" ht="210" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
         <v>349</v>
       </c>
@@ -9098,7 +9039,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>351</v>
       </c>
@@ -9124,7 +9065,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="207" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
         <v>352</v>
       </c>
@@ -9150,7 +9091,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="208" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:8" ht="150" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>353</v>
       </c>
@@ -9176,7 +9117,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="209" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:8" ht="195" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>355</v>
       </c>
@@ -9202,7 +9143,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="210" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>357</v>
       </c>
@@ -9228,7 +9169,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="211" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>359</v>
       </c>
@@ -9254,7 +9195,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="212" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>361</v>
       </c>
@@ -9280,7 +9221,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="213" spans="1:8" ht="240" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>363</v>
       </c>
@@ -9306,7 +9247,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="214" spans="1:8" ht="409" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:8" ht="240" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
         <v>365</v>
       </c>

</xml_diff>

<commit_message>
1. support time based keywords in date parsing 2. smart fill of smart/end date year 3. return only start date in case of 1 grepped date
</commit_message>
<xml_diff>
--- a/data_utils/data_for_tagging.xlsx
+++ b/data_utils/data_for_tagging.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avishaya\PycharmProjects\traveliz\data_utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4D44A3-1C47-4B9F-B48C-06A9A2EE4893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD834ED-439C-440C-889C-99874FD1C3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="facebook" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2229" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2229" uniqueCount="660">
   <si>
     <t>Post_id</t>
   </si>
@@ -3337,6 +3337,15 @@
   </si>
   <si>
     <t>3 s</t>
+  </si>
+  <si>
+    <t>18.12.2021</t>
+  </si>
+  <si>
+    <t>6.12.2021</t>
+  </si>
+  <si>
+    <t>5.12.2021</t>
   </si>
 </sst>
 </file>
@@ -4630,8 +4639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H214"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6001,10 +6010,10 @@
         <v>190</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>16</v>
+        <v>659</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>17</v>
+        <v>658</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>18</v>
@@ -6394,7 +6403,7 @@
         <v>134</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>80</v>
+        <v>657</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>18</v>
@@ -10423,8 +10432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>